<commit_message>
TS02 code added [party functionality]
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -3,37 +3,36 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0FFC61C6-1449-4BFE-95BB-D085C29B26D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{41B9FD17-6442-4171-A0AC-48DB21D80ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Case Master-OLD" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Case Master" sheetId="2" r:id="rId2"/>
-    <sheet name="Basic Details" sheetId="3" r:id="rId3"/>
-    <sheet name="Accounts" sheetId="4" r:id="rId4"/>
-    <sheet name="Party" sheetId="5" r:id="rId5"/>
-    <sheet name="Budget" sheetId="6" r:id="rId6"/>
-    <sheet name="Scheduled" sheetId="7" r:id="rId7"/>
-    <sheet name="Payment Profile" sheetId="8" r:id="rId8"/>
+    <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Accounts" sheetId="3" r:id="rId3"/>
+    <sheet name="Party" sheetId="4" r:id="rId4"/>
+    <sheet name="Budget" sheetId="5" r:id="rId5"/>
+    <sheet name="Scheduled" sheetId="6" r:id="rId6"/>
+    <sheet name="Payment Profile" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K4"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7miJVWP15JaCovKwi0Jx2gEs/j/q6Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7miN0ZB4aP7dq/8ubycJJfJNbm6Mag=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="146">
-  <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
-    <t>Skip</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="140">
+  <si>
+    <t>Test Scenario ID</t>
+  </si>
+  <si>
+    <t>Run TC</t>
   </si>
   <si>
     <t>Module name</t>
@@ -43,59 +42,6 @@
   </si>
   <si>
     <t>Assertion</t>
-  </si>
-  <si>
-    <t>TC03</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Basic Deatils</t>
-  </si>
-  <si>
-    <t>Create a Deal having Accounts for XCRO Transactions</t>
-  </si>
-  <si>
-    <t>TC01</t>
-  </si>
-  <si>
-    <t>Accounts</t>
-  </si>
-  <si>
-    <t>Create a Deal having Accounts, Parties for EComm Transactions</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>Create a XCRO Deal having 2 Payments</t>
-  </si>
-  <si>
-    <t>Budget</t>
-  </si>
-  <si>
-    <t>Create a XCRO Deal with 1 Retention and 2 Payments</t>
-  </si>
-  <si>
-    <t>In the Budget Screen, validate the Available Budget and Utilized budget</t>
-  </si>
-  <si>
-    <t>TC100</t>
-  </si>
-  <si>
-    <t>Create Deal Basic details info and select Contexualize
-Onboarding a account
-Creating a payment with PRS</t>
-  </si>
-  <si>
-    <t>TC02</t>
-  </si>
-  <si>
-    <t>Test Scenario ID</t>
-  </si>
-  <si>
-    <t>Run TC</t>
   </si>
   <si>
     <t>TS01</t>
@@ -106,6 +52,9 @@
   <si>
     <t>Basic Details
 Accounts</t>
+  </si>
+  <si>
+    <t>Create a Deal having Accounts for XCRO Transactions</t>
   </si>
   <si>
     <t>TS02</t>
@@ -116,14 +65,21 @@
 Party</t>
   </si>
   <si>
+    <t>Create a Deal having Accounts,Basicdetails, Parties</t>
+  </si>
+  <si>
     <t>TS03</t>
   </si>
   <si>
     <t>Basic Details
 Accounts
 Party
-Payments
-Retention</t>
+Payments</t>
+  </si>
+  <si>
+    <t>Create Deal Basic details info
+Onboarding a account
+Creating a payment</t>
   </si>
   <si>
     <t>TS04</t>
@@ -132,17 +88,31 @@
     <t>Basic Details
 Accounts
 Party
-Payments
-Retention
-Fees</t>
+Linked Instruction</t>
+  </si>
+  <si>
+    <t>Create a XCRO Deal as TS03 + Linked Instruction payment</t>
+  </si>
+  <si>
+    <t>TS05</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Basic Details
+Accounts
+Party
+Budget
+Scheduled payment</t>
+  </si>
+  <si>
+    <t>TS03 + Budget and Payments</t>
   </si>
   <si>
     <t>In the Budget Screen, validate the Available Budget and Utilized budget next day</t>
   </si>
   <si>
-    <t>TS05</t>
-  </si>
-  <si>
     <t>Deal Name</t>
   </si>
   <si>
@@ -215,9 +185,6 @@
     <t>TS02_Deal</t>
   </si>
   <si>
-    <t>flexible funding</t>
-  </si>
-  <si>
     <t>Mumbai HO</t>
   </si>
   <si>
@@ -227,9 +194,6 @@
     <t>Singapore</t>
   </si>
   <si>
-    <t>Acquirer</t>
-  </si>
-  <si>
     <t>BT</t>
   </si>
   <si>
@@ -257,9 +221,27 @@
     <t>Physical</t>
   </si>
   <si>
+    <t>Country Code</t>
+  </si>
+  <si>
     <t>INR</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
     <t>Add a new Party</t>
   </si>
   <si>
@@ -324,9 +306,6 @@
   </si>
   <si>
     <t>BIC123</t>
-  </si>
-  <si>
-    <t>IN</t>
   </si>
   <si>
     <t>SBI98765</t>
@@ -391,7 +370,7 @@
     <t>Select Instruction Type</t>
   </si>
   <si>
-    <t>Basic Deatils - Name</t>
+    <t>Basic Details Name</t>
   </si>
   <si>
     <t>Balance Consideration</t>
@@ -479,13 +458,16 @@
 Debit Remittance Info</t>
   </si>
   <si>
-    <t>SG</t>
-  </si>
-  <si>
     <t>TT</t>
   </si>
   <si>
-    <t>Country Code</t>
+    <t>Movie Production</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -495,10 +477,50 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -511,20 +533,26 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -554,36 +582,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -804,7 +850,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1001"/>
+  <dimension ref="A1:F992"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -814,8 +860,9 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="57.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
@@ -852,208 +899,125 @@
       <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="8"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="8"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="8"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="2"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="8"/>
+      <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2014,15 +1978,6 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,1149 +1988,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F993"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="80.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:M1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3191,182 +2008,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="M1" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="2"/>
+      <c r="A3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="16">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="D4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="A5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="A6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4367,101 +3188,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>145</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
+      <c r="A2" s="17" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>94</v>
+        <v>40</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
+      <c r="A3" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>94</v>
+        <v>49</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>27</v>
+      <c r="A4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:S998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4473,134 +3318,135 @@
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="I1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="K1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="L1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="M1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="N1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="O1" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="P1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="Q1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="R1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="S1" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="S2" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>27</v>
+      <c r="A3" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
+      <c r="A4" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5602,8 +4448,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5620,78 +4466,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="J1" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>37</v>
+      <c r="K1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="12">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="18">
         <v>1000</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="19">
         <v>44958</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="19">
         <v>44958</v>
       </c>
     </row>
@@ -5700,8 +4546,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5725,151 +4571,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="L1" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="M1" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="N1" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="O1" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="P1" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="Q1" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="R1" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="S1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="U1" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="V1" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="R2" s="12">
+      <c r="H2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" s="18">
         <v>400</v>
       </c>
-      <c r="S2" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>6</v>
+      <c r="S2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5887,40 +4733,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>142</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>62</v>
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>144</v>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Completed Transaction maker and checker flow
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9084" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="154">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>TS04_Deal</t>
+  </si>
+  <si>
+    <t>At specific time</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,6 +698,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2055,8 +2061,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2271,7 +2277,9 @@
       <c r="L6" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="30"/>
+    </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3266,6 +3274,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3276,7 +3285,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5:E5"/>
     </sheetView>
@@ -4866,7 +4875,9 @@
   </sheetPr>
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4991,7 +5002,7 @@
         <v>101</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
Started Test case 07 ECommerce Transaction (Deal with eComm Party, Ecomm Transaction Maker, Checker and Approver)
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ManishaDrive1\Appveen\FinalFramework\upp-test-automation\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12924" windowHeight="5208" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="7296" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,6 @@
     <sheet name="Payment Profile" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I15"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId21" roundtripDataSignature="AMtx7mhutaEAu3Eo/TVBwvxT6q/0+D6ZAw=="/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="231">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -472,15 +476,6 @@
     <t>Current Date</t>
   </si>
   <si>
-    <t>TestUser4</t>
-  </si>
-  <si>
-    <t>Testuser4@gmail.com</t>
-  </si>
-  <si>
-    <t>BIC678</t>
-  </si>
-  <si>
     <t>TestUser5</t>
   </si>
   <si>
@@ -757,6 +752,18 @@
   </si>
   <si>
     <t>TT</t>
+  </si>
+  <si>
+    <t>TS07_Deal</t>
+  </si>
+  <si>
+    <t>TestUser7</t>
+  </si>
+  <si>
+    <t>Testuser7@gmail.com</t>
+  </si>
+  <si>
+    <t>Testuser4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -766,7 +773,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -834,6 +841,13 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -892,10 +906,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -978,8 +993,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1200,7 +1217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2425,13 +2442,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2439,13 +2456,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2500,67 +2517,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>107</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>89</v>
       </c>
       <c r="F1" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="N1" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>204</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="N1" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>207</v>
       </c>
       <c r="P1" s="31" t="s">
         <v>113</v>
       </c>
       <c r="Q1" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="R1" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="S1" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="U1" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="U1" s="31" t="s">
-        <v>184</v>
-      </c>
       <c r="V1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -2568,25 +2585,25 @@
         <v>29</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>95</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>80</v>
@@ -2595,22 +2612,22 @@
         <v>79</v>
       </c>
       <c r="K2" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="N2" s="31" t="s">
         <v>211</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>214</v>
       </c>
       <c r="O2" s="31" t="s">
         <v>56</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q2" s="31">
         <v>250</v>
@@ -2619,16 +2636,16 @@
         <v>80</v>
       </c>
       <c r="S2" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="U2" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="T2" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="U2" s="31" t="s">
-        <v>192</v>
-      </c>
       <c r="V2" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2657,13 +2674,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,13 +2688,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2701,13 +2718,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2715,13 +2732,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2759,7 +2776,7 @@
         <v>103</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>105</v>
@@ -2768,7 +2785,7 @@
         <v>42</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>110</v>
@@ -2798,10 +2815,10 @@
         <v>118</v>
       </c>
       <c r="R1" s="31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,13 +2829,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>121</v>
@@ -2827,13 +2844,13 @@
         <v>53</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>54</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K2" s="31" t="s">
         <v>123</v>
@@ -2845,7 +2862,7 @@
         <v>80</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O2" s="31" t="s">
         <v>79</v>
@@ -2857,10 +2874,10 @@
         <v>127</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2888,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2899,10 +2916,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2933,16 +2950,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>225</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2962,7 +2979,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3975,7 +3992,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4247,7 +4264,43 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="27">
+        <v>1</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" s="35"/>
+    </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5250,11 +5303,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5380,6 +5433,23 @@
       </c>
       <c r="E7" s="18" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -5493,7 +5563,9 @@
   </sheetPr>
   <dimension ref="A1:T998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5691,54 +5763,59 @@
       <c r="A4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>71</v>
+        <v>55</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>121</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>7</v>
+      </c>
       <c r="J4" s="31" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>137</v>
+        <v>54</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>230</v>
       </c>
       <c r="M4" s="31" t="s">
         <v>123</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P4" s="31" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="T4" s="31" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5749,34 +5826,34 @@
         <v>7</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>54</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>54</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>123</v>
@@ -5808,34 +5885,34 @@
         <v>7</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>71</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>70</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K6" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M6" s="31" t="s">
         <v>123</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>84</v>
@@ -5853,7 +5930,65 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="S7" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6846,6 +6981,10 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1"/>
+    <hyperlink ref="L4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6879,10 +7018,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>89</v>
@@ -6891,55 +7030,55 @@
         <v>86</v>
       </c>
       <c r="F1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="N1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="Q1" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>157</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>160</v>
       </c>
       <c r="S1" s="31" t="s">
         <v>113</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="U1" s="31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="V1" s="31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -6947,19 +7086,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>23</v>
@@ -6977,10 +7116,10 @@
         <v>135</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>94</v>
@@ -6998,7 +7137,7 @@
         <v>400</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="T2" s="31" t="s">
         <v>84</v>
@@ -7025,8 +7164,8 @@
   </sheetPr>
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7042,10 +7181,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>89</v>
@@ -7054,61 +7193,61 @@
         <v>86</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J1" s="31" t="s">
         <v>90</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="S1" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="T1" s="31" t="s">
         <v>157</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>160</v>
       </c>
       <c r="U1" s="31" t="s">
         <v>113</v>
       </c>
       <c r="V1" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="W1" s="31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="X1" s="31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -7116,19 +7255,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>23</v>
@@ -7137,10 +7276,10 @@
         <v>23</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K2" s="35" t="s">
         <v>7</v>
@@ -7152,10 +7291,10 @@
         <v>135</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P2" s="35" t="s">
         <v>51</v>
@@ -7173,7 +7312,7 @@
         <v>500</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="V2" s="35" t="s">
         <v>80</v>
@@ -7215,13 +7354,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>89</v>
@@ -7230,37 +7369,37 @@
         <v>86</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="I1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="J1" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="M1" s="34" t="s">
+      <c r="P1" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="31" t="s">
         <v>182</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -7268,16 +7407,16 @@
         <v>27</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>95</v>
@@ -7286,7 +7425,7 @@
         <v>70</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>123</v>
@@ -7301,19 +7440,19 @@
         <v>84</v>
       </c>
       <c r="M2" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="Q2" s="31" t="s">
         <v>190</v>
-      </c>
-      <c r="O2" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="P2" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -7345,13 +7484,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7359,13 +7498,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Payment Transaction to TS09.
Added Payment Transaction to TS09.
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -28,14 +28,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mj0upXukzQjdXcZMoA76U6LD7wfHQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mgG4Sl0IX8+8z1LblT6PwhF9HRwcA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="287">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -315,7 +315,13 @@
     <t>TS05_Deal</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>TS06_Deal</t>
+  </si>
+  <si>
+    <t>TS07_Deal</t>
   </si>
   <si>
     <t>TS09_Deal</t>
@@ -408,6 +414,15 @@
   </si>
   <si>
     <t>Feb</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Phone Bill</t>
+  </si>
+  <si>
+    <t>Monthly</t>
   </si>
   <si>
     <t>Add a new Party</t>
@@ -639,10 +654,37 @@
     <t>Next Business Day</t>
   </si>
   <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>At specific time</t>
+  </si>
+  <si>
+    <t>Bill Payment</t>
+  </si>
+  <si>
+    <t>Ledger Balance</t>
+  </si>
+  <si>
+    <t>Do not execute on holiday</t>
+  </si>
+  <si>
+    <t>ICICI178</t>
+  </si>
+  <si>
     <t>Parent Test case</t>
   </si>
   <si>
-    <t>API Payload</t>
+    <t>PArty Type</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>PAyload</t>
   </si>
   <si>
     <t>TS12-1</t>
@@ -654,10 +696,160 @@
     <t xml:space="preserve"> Individual</t>
   </si>
   <si>
+    <t>https://dev.upp.appveen.com/mdm/api/party</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>{
+        "party": {
+                "dealRefId": "REF1672297910549",
+                "name": "Ranjith123",
+                "partyRefId": "Ranjith123",
+                "country": "IN",
+                "status": "Active",
+                "kycCompleted": true,
+                "validFrom": "2021-09-17",
+                "validUntil": "2023-12-31",
+                "responsibility": "Acquiree",
+                "attributes": {
+                        "acquiree": "Merchant",
+                        "number": 10
+                },
+"type":"company",
+"company":{
+"incorporationDate":"2021-09-17",
+"registrationNumber":"REG123432",
+"taxId":"",
+"taxType":"",
+"businessCategory":"",
+"businessType":"",
+"listingAuthority":""
+},
+                "executionPolicies": {
+                        "onPartyActivate": "doNothing",
+                        "onPartyDeactivate": "holdExecutions"
+                },
+                "contacts": [{
+                        "name": "Merchant33",
+                        "designation": "Manager",
+                        "authorizedSignatory": false,
+                        "enableNotifications": false,
+                        "workPhone": "+91 92392 29932",
+                        "mobilePhone": "+91 92392 29932",
+                        "email": "jane.doe@gmail.com",
+                        "address": {
+                                "town": "Bengaluru Urban",
+                                "street": "M G Road",
+                                "zip_pin": "4000340",
+                                "state": "KA",
+                                "country": "IN"
+                        }
+                }],
+                "accounts": [{
+                        "paymentInstrumentId": "AK-Pay",
+                        "description": "Payout Account",
+                        "paymentDetails": {
+                                "accountIban": "Account Number",
+                                "to": "123123122133",
+                                "receiverPop": "123",
+                                "name": "Merchant293",
+                                "beneficiaryCountry": "IN",
+                                "beneficiaryCurrency": "INR"
+                        },
+            "overrides": [{
+                    "profileName": "Payment Profile",
+                    "paymentInstrument":"BT",
+                    "country": "IN",
+                    "attributes": [
+                        {
+                            "name": "Charge Bearer",
+                            "value": "SHA"
+                        }
+                    ]
+                }]
+                }]
+        }
+}</t>
+  </si>
+  <si>
     <t>TS12-2</t>
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>{
+        "party": {
+                "dealRefId": "REF1672297910549",
+                "name": "Karthik123",
+                "partyRefId": "Karthik123",
+                "country": "IN",
+                "status": "Active",
+                "kycCompleted": true,
+                "validFrom": "2021-09-17",
+                "validUntil": "2023-12-31",
+                "responsibility": "Acquiree",
+                "attributes": {
+                        "acquiree": "Merchant",
+                        "number": 10
+                },
+"type":"company",
+"company":{
+"incorporationDate":"2021-09-17",
+"registrationNumber":"REG123432",
+"taxId":"",
+"taxType":"",
+"businessCategory":"",
+"businessType":"",
+"listingAuthority":""
+},
+                "executionPolicies": {
+                        "onPartyActivate": "doNothing",
+                        "onPartyDeactivate": "holdExecutions"
+                },
+                "contacts": [{
+                        "name": "Merchant33",
+                        "designation": "Manager",
+                        "authorizedSignatory": false,
+                        "enableNotifications": false,
+                        "workPhone": "+91 92392 29932",
+                        "mobilePhone": "+91 92392 29932",
+                        "email": "jane.doe@gmail.com",
+                        "address": {
+                                "town": "Bengaluru Urban",
+                                "street": "M G Road",
+                                "zip_pin": "4000340",
+                                "state": "KA",
+                                "country": "IN"
+                        }
+                }],
+                "accounts": [{
+                        "paymentInstrumentId": "AK-Pay",
+                        "description": "Payout Account",
+                        "paymentDetails": {
+                                "accountIban": "Account Number",
+                                "to": "123123122133",
+                                "receiverPop": "123",
+                                "name": "Merchant293",
+                                "beneficiaryCountry": "IN",
+                                "beneficiaryCurrency": "INR"
+                        },
+            "overrides": [{
+                    "profileName": "Payment Profile",
+                    "paymentInstrument":"BT",
+                    "country": "IN",
+                    "attributes": [
+                        {
+                            "name": "Charge Bearer",
+                            "value": "SHA"
+                        }
+                    ]
+                }]
+                }]
+        }
+}</t>
   </si>
   <si>
     <t>Linked - Amount</t>
@@ -676,9 +868,6 @@
     <t>Disabled</t>
   </si>
   <si>
-    <t>At specific time</t>
-  </si>
-  <si>
     <t>CREATE TRANSACTION - Deal Ref Id</t>
   </si>
   <si>
@@ -695,9 +884,6 @@
   </si>
   <si>
     <t>Documents-Document Type</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
   <si>
     <t>File Type</t>
@@ -896,8 +1082,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd-mmm-yyyy"/>
+    <numFmt numFmtId="165" formatCode="mmm-d"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -949,12 +1136,12 @@
       <name val="Verdana"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1008,7 +1195,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1114,6 +1301,15 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -1123,17 +1319,11 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -29417,52 +29607,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" s="35" t="s">
-        <v>207</v>
-      </c>
       <c r="O1" s="35" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -29470,52 +29660,52 @@
         <v>27</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>76</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="K2" s="35">
         <v>500.0</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29546,13 +29736,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -29560,13 +29750,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29594,13 +29784,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -29608,13 +29798,13 @@
         <v>27</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29667,67 +29857,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F1" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="T1" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="35" t="s">
+      <c r="U1" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="V1" s="35" t="s">
         <v>226</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>231</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>232</v>
-      </c>
-      <c r="P1" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="S1" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="V1" s="35" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="2">
@@ -29735,67 +29925,67 @@
         <v>29</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="O2" s="35" t="s">
         <v>62</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="Q2" s="35">
         <v>250.0</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29823,13 +30013,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -29837,13 +30027,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29866,13 +30056,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -29880,13 +30070,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -29915,58 +30105,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E1" s="35" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G1" s="35" t="s">
         <v>48</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -29977,55 +30167,55 @@
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -30052,10 +30242,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
@@ -30063,10 +30253,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -30094,46 +30284,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2">
@@ -30141,46 +30331,46 @@
         <v>36</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="K2" s="38">
         <v>44991.0</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -30403,8 +30593,8 @@
       <c r="B6" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>66</v>
+      <c r="C6" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>67</v>
@@ -30416,8 +30606,8 @@
       <c r="G6" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>70</v>
+      <c r="H6" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="I6" s="26" t="s">
         <v>60</v>
@@ -30435,7 +30625,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="35">
         <v>1.0</v>
@@ -30469,6 +30659,36 @@
       <c r="A8" s="34" t="s">
         <v>29</v>
       </c>
+      <c r="B8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
@@ -30480,13 +30700,13 @@
         <v>33</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C10" s="35">
         <v>1.0</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>56</v>
@@ -30495,7 +30715,7 @@
         <v>57</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>59</v>
@@ -30504,7 +30724,7 @@
         <v>76</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K10" s="28" t="s">
         <v>78</v>
@@ -31531,16 +31751,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -31548,19 +31768,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -32590,13 +32810,13 @@
         <v>48</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
@@ -32607,13 +32827,13 @@
         <v>59</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
@@ -32624,13 +32844,13 @@
         <v>70</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
@@ -32641,13 +32861,13 @@
         <v>75</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
@@ -32658,13 +32878,13 @@
         <v>59</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
@@ -32672,7 +32892,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>91</v>
@@ -32692,13 +32912,13 @@
         <v>75</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
@@ -32719,13 +32939,13 @@
         <v>59</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
@@ -32760,31 +32980,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K1" s="35" t="s">
         <v>45</v>
@@ -32798,28 +33018,28 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J2" s="35">
         <v>1000.0</v>
@@ -32830,6 +33050,32 @@
       <c r="L2" s="38">
         <v>44958.0</v>
       </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="40">
+        <v>45130.0</v>
+      </c>
+      <c r="J3" s="41">
+        <v>1000.0</v>
+      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -32863,61 +33109,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -32928,55 +33174,55 @@
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>60</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="K2" s="35" t="s">
         <v>60</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -32987,53 +33233,53 @@
         <v>7</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>76</v>
       </c>
       <c r="H3" s="35"/>
       <c r="J3" s="35" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>76</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="R3" s="35" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -33044,10 +33290,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>77</v>
@@ -33057,37 +33303,37 @@
       </c>
       <c r="H4" s="35"/>
       <c r="J4" s="35" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="K4" s="35" t="s">
         <v>76</v>
       </c>
       <c r="L4" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="M4" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="N4" s="35" t="s">
+      <c r="Q4" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="R4" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="O4" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="R4" s="35" t="s">
-        <v>144</v>
-      </c>
       <c r="S4" s="35" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -33098,55 +33344,55 @@
         <v>7</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>61</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>60</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="K5" s="35" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P5" s="35" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="Q5" s="35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -33157,49 +33403,49 @@
         <v>7</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="K6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P6" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="S6" s="35" t="s">
         <v>143</v>
-      </c>
-      <c r="Q6" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -33220,52 +33466,52 @@
         <v>7</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>157</v>
+        <v>162</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>162</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="G9" s="35" t="s">
         <v>76</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K9" s="35" t="s">
         <v>60</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="40" t="s">
-        <v>160</v>
+        <v>139</v>
+      </c>
+      <c r="N9" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P9" s="35" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="Q9" s="35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R9" s="35" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="S9" s="35" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="T9" s="35" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -34281,7 +34527,7 @@
     <col customWidth="1" min="3" max="3" width="18.75"/>
     <col customWidth="1" min="6" max="6" width="17.88"/>
     <col customWidth="1" min="10" max="10" width="20.25"/>
-    <col customWidth="1" min="13" max="13" width="16.13"/>
+    <col customWidth="1" min="13" max="13" width="20.25"/>
     <col customWidth="1" min="15" max="15" width="10.0"/>
     <col customWidth="1" min="16" max="16" width="22.63"/>
     <col customWidth="1" min="19" max="19" width="16.88"/>
@@ -34295,67 +34541,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>172</v>
+        <v>176</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>177</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2">
@@ -34363,67 +34609,61 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>184</v>
-      </c>
-      <c r="N2" s="35" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="P2" s="35" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="R2" s="35">
         <v>400.0</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
@@ -34431,67 +34671,197 @@
         <v>39</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="R3" s="35">
         <v>400.0</v>
       </c>
       <c r="S3" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="U3" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="V3" s="35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="T3" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="35" t="s">
+      <c r="C4" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="F4" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="N4" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="P4" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q4" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="R4" s="41">
+        <v>600.0</v>
+      </c>
+      <c r="S4" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="T4" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="U4" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="V4" s="39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>107</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="R5" s="35">
+        <v>17800.0</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="U5" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -34511,6 +34881,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="17.88"/>
     <col customWidth="1" min="2" max="2" width="23.38"/>
+    <col customWidth="1" min="4" max="4" width="37.38"/>
+    <col customWidth="1" min="6" max="6" width="65.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -34518,36 +34890,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>200</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" ht="258.0" customHeight="1">
       <c r="A2" s="35" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>192</v>
+        <v>206</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>194</v>
+        <v>211</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -34586,147 +34982,147 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>196</v>
+        <v>102</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>214</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>172</v>
+        <v>176</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>177</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" s="43" t="s">
+      <c r="B2" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="K2" s="43" t="s">
+      <c r="F2" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="N2" s="43" t="s">
-        <v>200</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="P2" s="43" t="s">
+      <c r="L2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="P2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="R2" s="43" t="s">
+      <c r="Q2" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="43" t="s">
+      <c r="S2" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="T2" s="41">
+        <v>500.0</v>
+      </c>
+      <c r="U2" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="V2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="T2" s="44">
-        <v>500.0</v>
-      </c>
-      <c r="U2" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="V2" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="W2" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="X2" s="43" t="s">
-        <v>107</v>
+      <c r="X2" s="39" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded latest Excel sheet from Google drive,Added TS09 and TS11
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -757,9 +757,9 @@
   <si>
     <t>{
         "party": {
-                "dealRefId": "REF1678164931132",
-                "name": "Party12345678",
-                "partyRefId": "Party12345670",
+                "dealRefId": "REF1678428748624",
+                "name": "Party1234567809",
+                "partyRefId": "Party1234567009",
                 "country": "IN",
                 "status": "Active",
                 "kycCompleted": true,
@@ -804,7 +804,8 @@
                         "beneficiaryCountry":"IN",
                         "beneficiaryCurrency":"INR",
                         "to":"SBI98765",
-                        "beneficiaryCountryOfIncorporation":"IN"
+                        "beneficiaryCountryOfIncorporation":"IN",
+                        "amount":1000
                         }
                 }]
         }

</xml_diff>

<commit_message>
E-commerce transaction flow completed
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\dev\upp-test-automation\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,6 @@
     <sheet name="Payment Profile" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H15"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mgG4Sl0IX8+8z1LblT6PwhF9HRwcA=="/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="302">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -141,6 +145,9 @@
     <t>TS05-Assertion</t>
   </si>
   <si>
+    <t>Assertion for Budget details</t>
+  </si>
+  <si>
     <t>In the Budget Screen, validate the Available Budget and Utilized budget next day</t>
   </si>
   <si>
@@ -192,14 +199,28 @@
     <t>a) Creating a Holiday for Future date (Ex: 06-March-2023) and [TS03] creating a SCHD txn for the same date and because of holiday Action(next business day), txn should be schd for 07-March-2023 and executed on the same date</t>
   </si>
   <si>
-    <t>TS03-assertion1</t>
+    <t>TS10-assertion1</t>
   </si>
   <si>
-    <t>TS10- Assertion for TS 10</t>
+    <t>Assertion for TS 10</t>
   </si>
   <si>
     <t>As per the Holiday Configuration and Holiday action, transaction should be created and executed accordingly.
 Note: Validate the txn schd date</t>
+  </si>
+  <si>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>Basic Details
+Accounts
+Party
+Payments
+(AND)
+PARTY API</t>
+  </si>
+  <si>
+    <t>TS03 + Add Party through Api and creating a txn</t>
   </si>
   <si>
     <t>Deal Name</t>
@@ -319,7 +340,13 @@
     <t>TS05_Deal</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>TS06_Deal</t>
+  </si>
+  <si>
+    <t>TS07_Deal</t>
   </si>
   <si>
     <t>TS09_Deal</t>
@@ -332,6 +359,15 @@
   </si>
   <si>
     <t>Acquirer</t>
+  </si>
+  <si>
+    <t>TS10_Deal_Holiday</t>
+  </si>
+  <si>
+    <t>TS011_Deal</t>
+  </si>
+  <si>
+    <t>ALL</t>
   </si>
   <si>
     <t>Currency</t>
@@ -558,6 +594,12 @@
     <t>BICTS06</t>
   </si>
   <si>
+    <t>TestUser7</t>
+  </si>
+  <si>
+    <t>Testuser7@gmail.com</t>
+  </si>
+  <si>
     <t>TestUser9</t>
   </si>
   <si>
@@ -571,6 +613,21 @@
   </si>
   <si>
     <t>IMDTS09</t>
+  </si>
+  <si>
+    <t>TestUser11</t>
+  </si>
+  <si>
+    <t>Test11 remarks</t>
+  </si>
+  <si>
+    <t>Testuser11@gmail.com</t>
+  </si>
+  <si>
+    <t>BICTS11</t>
+  </si>
+  <si>
+    <t>IMDTS11</t>
   </si>
   <si>
     <t>Select Instruction Type</t>
@@ -646,6 +703,9 @@
     <t>SCBASDFGH</t>
   </si>
   <si>
+    <t>TS03-assertion1</t>
+  </si>
+  <si>
     <t>March 06-2023</t>
   </si>
   <si>
@@ -655,10 +715,31 @@
     <t>Bill</t>
   </si>
   <si>
+    <t>At specific time</t>
+  </si>
+  <si>
+    <t>Bill Payment</t>
+  </si>
+  <si>
+    <t>Ledger Balance</t>
+  </si>
+  <si>
+    <t>Do not execute on holiday</t>
+  </si>
+  <si>
+    <t>ICICI178</t>
+  </si>
+  <si>
+    <t>TS11 Payment</t>
+  </si>
+  <si>
+    <t>SBITS11</t>
+  </si>
+  <si>
     <t>Parent Test case</t>
   </si>
   <si>
-    <t>PArty Type</t>
+    <t>Party Type</t>
   </si>
   <si>
     <t>URL</t>
@@ -667,16 +748,13 @@
     <t>Method</t>
   </si>
   <si>
-    <t>PAyload</t>
+    <t>Payload</t>
   </si>
   <si>
-    <t>TS12-1</t>
+    <t>TS11-1</t>
   </si>
   <si>
-    <t>TS12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Individual</t>
+    <t>Company</t>
   </si>
   <si>
     <t>https://dev.upp.appveen.com/mdm/api/party</t>
@@ -687,19 +765,15 @@
   <si>
     <t>{
         "party": {
-                "dealRefId": "REF1672297910549",
-                "name": "Ranjith123",
-                "partyRefId": "Ranjith123",
+                "dealRefId": "REF1678164931132",
+                "name": "Party12345678",
+                "partyRefId": "Party12345670",
                 "country": "IN",
                 "status": "Active",
                 "kycCompleted": true,
                 "validFrom": "2021-09-17",
                 "validUntil": "2023-12-31",
                 "responsibility": "Acquiree",
-                "attributes": {
-                        "acquiree": "Merchant",
-                        "number": 10
-                },
 "type":"company",
 "company":{
 "incorporationDate":"2021-09-17",
@@ -731,108 +805,24 @@
                         }
                 }],
                 "accounts": [{
-                        "paymentInstrumentId": "AK-Pay",
+                        "paymentInstrumentId": "BT",
                         "description": "Payout Account",
                         "paymentDetails": {
-                                "accountIban": "Account Number",
-                                "to": "123123122133",
-                                "receiverPop": "123",
-                                "name": "Merchant293",
-                                "beneficiaryCountry": "IN",
-                                "beneficiaryCurrency": "INR"
-                        },
-            "overrides": [{
-                    "profileName": "Payment Profile",
-                    "paymentInstrument":"BT",
-                    "country": "IN",
-                    "attributes": [
-                        {
-                            "name": "Charge Bearer",
-                            "value": "SHA"
+                        "beneficiaryBankBic": "BIC456",
+                        "beneficiaryCountry":"IN",
+                        "beneficiaryCurrency":"INR",
+                        "to":"SBI98765",
+                        "beneficiaryCountryOfIncorporation":"IN"
                         }
-                    ]
-                }]
                 }]
         }
 }</t>
   </si>
   <si>
-    <t>TS12-2</t>
+    <t>TS11-2</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>{
-        "party": {
-                "dealRefId": "REF1672297910549",
-                "name": "Karthik123",
-                "partyRefId": "Karthik123",
-                "country": "IN",
-                "status": "Active",
-                "kycCompleted": true,
-                "validFrom": "2021-09-17",
-                "validUntil": "2023-12-31",
-                "responsibility": "Acquiree",
-                "attributes": {
-                        "acquiree": "Merchant",
-                        "number": 10
-                },
-"type":"company",
-"company":{
-"incorporationDate":"2021-09-17",
-"registrationNumber":"REG123432",
-"taxId":"",
-"taxType":"",
-"businessCategory":"",
-"businessType":"",
-"listingAuthority":""
-},
-                "executionPolicies": {
-                        "onPartyActivate": "doNothing",
-                        "onPartyDeactivate": "holdExecutions"
-                },
-                "contacts": [{
-                        "name": "Merchant33",
-                        "designation": "Manager",
-                        "authorizedSignatory": false,
-                        "enableNotifications": false,
-                        "workPhone": "+91 92392 29932",
-                        "mobilePhone": "+91 92392 29932",
-                        "email": "jane.doe@gmail.com",
-                        "address": {
-                                "town": "Bengaluru Urban",
-                                "street": "M G Road",
-                                "zip_pin": "4000340",
-                                "state": "KA",
-                                "country": "IN"
-                        }
-                }],
-                "accounts": [{
-                        "paymentInstrumentId": "AK-Pay",
-                        "description": "Payout Account",
-                        "paymentDetails": {
-                                "accountIban": "Account Number",
-                                "to": "123123122133",
-                                "receiverPop": "123",
-                                "name": "Merchant293",
-                                "beneficiaryCountry": "IN",
-                                "beneficiaryCurrency": "INR"
-                        },
-            "overrides": [{
-                    "profileName": "Payment Profile",
-                    "paymentInstrument":"BT",
-                    "country": "IN",
-                    "attributes": [
-                        {
-                            "name": "Charge Bearer",
-                            "value": "SHA"
-                        }
-                    ]
-                }]
-                }]
-        }
-}</t>
+    <t>Individual</t>
   </si>
   <si>
     <t>Linked - Amount</t>
@@ -849,9 +839,6 @@
   </si>
   <si>
     <t>Disabled</t>
-  </si>
-  <si>
-    <t>At specific time</t>
   </si>
   <si>
     <t>CREATE TRANSACTION - Deal Ref Id</t>
@@ -944,13 +931,7 @@
     <t>Fragment Platform Reference No</t>
   </si>
   <si>
-    <t>Instrument - category</t>
-  </si>
-  <si>
     <t>PartyABCD</t>
-  </si>
-  <si>
-    <t>Adhoc Payment1</t>
   </si>
   <si>
     <t>Creditorpartyid123</t>
@@ -974,7 +955,7 @@
     <t>Should be same as Ecomm Maker screen amount</t>
   </si>
   <si>
-    <t>TestUser100</t>
+    <t>TestUser1002</t>
   </si>
   <si>
     <t>Testuser100@gmail.com</t>
@@ -1064,7 +1045,10 @@
     <t>TT</t>
   </si>
   <si>
-    <t>Test</t>
+    <t xml:space="preserve">Payment </t>
+  </si>
+  <si>
+    <t>Instrument category</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1059,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1128,6 +1112,25 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1201,7 +1204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1247,9 +1250,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1290,6 +1295,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1297,8 +1303,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1521,17 +1533,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="57.21875" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -1770,10 +1782,14 @@
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="3"/>
@@ -1799,14 +1815,14 @@
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="11" t="s">
@@ -1835,18 +1851,18 @@
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1871,14 +1887,14 @@
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="11" t="s">
@@ -1907,16 +1923,16 @@
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="11" t="s">
@@ -1945,16 +1961,16 @@
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="9"/>
@@ -1978,22 +1994,24 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:26" ht="68.25" customHeight="1">
+      <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18" t="s">
-        <v>40</v>
+      <c r="D13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -2015,15 +2033,23 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -2045,13 +2071,13 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -2073,13 +2099,13 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -29498,15 +29524,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="8" width="18.33203125" customWidth="1"/>
+    <col min="7" max="8" width="18.21875" customWidth="1"/>
     <col min="9" max="9" width="23.109375" customWidth="1"/>
     <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -29514,105 +29540,105 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>217</v>
+        <v>195</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>238</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="K2" s="35">
         <v>500</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="N2" s="45" t="s">
-        <v>225</v>
+        <v>245</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>246</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -29632,11 +29658,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29644,27 +29670,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -29681,11 +29707,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29693,27 +29719,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -29730,7 +29756,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29743,14 +29769,16 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
     <col min="8" max="8" width="23.109375" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
@@ -29768,139 +29796,140 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="K1" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="U1" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="V1" s="35" t="s">
         <v>241</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>242</v>
-      </c>
-      <c r="P1" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="S1" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="V1" s="35" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="E2" s="35" t="s">
         <v>244</v>
       </c>
+      <c r="E2" s="48" t="s">
+        <v>300</v>
+      </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="Q2" s="35">
         <v>250</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29913,11 +29942,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29925,27 +29954,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -29962,34 +29991,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -30006,12 +30035,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1">
@@ -30019,117 +30048,117 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>59</v>
+        <v>144</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>63</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -30146,10 +30175,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -30157,21 +30186,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -30188,11 +30217,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -30200,93 +30229,93 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="K2" s="38">
         <v>44991</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -30301,20 +30330,18 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="6" width="12.5546875" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.44140625" customWidth="1"/>
     <col min="8" max="10" width="16.88671875" customWidth="1"/>
     <col min="11" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
     <col min="13" max="13" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30323,40 +30350,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -30364,40 +30391,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C2" s="22">
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -30405,30 +30432,30 @@
         <v>10</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L3" s="27"/>
     </row>
@@ -30437,34 +30464,34 @@
         <v>14</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C4" s="26">
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L4" s="27"/>
     </row>
@@ -30473,34 +30500,34 @@
         <v>18</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C5" s="30">
         <v>1</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L5" s="32"/>
       <c r="M5" s="33"/>
@@ -30510,121 +30537,214 @@
         <v>22</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>281</v>
+        <v>84</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>85</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C7" s="35">
         <v>1</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C10" s="35">
         <v>1</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J10" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1"/>
+      <c r="D11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="14" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="15" spans="1:13" ht="15.75" customHeight="1"/>
@@ -31627,13 +31747,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -31641,16 +31761,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -31658,19 +31778,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1"/>
@@ -32680,17 +32800,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -32698,16 +32818,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -32715,16 +32835,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -32732,16 +32852,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -32749,16 +32869,16 @@
         <v>14</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -32766,16 +32886,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -32783,65 +32903,94 @@
         <v>22</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -32858,11 +33007,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="22.44140625" customWidth="1"/>
     <col min="10" max="10" width="20.109375" customWidth="1"/>
   </cols>
@@ -32872,37 +33021,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -32910,28 +33059,28 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="J2" s="35">
         <v>1000</v>
@@ -32948,17 +33097,17 @@
         <v>22</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="39" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I3" s="40">
         <v>45130</v>
@@ -32979,89 +33128,87 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T998"/>
+  <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="12.5546875" customWidth="1"/>
+    <col min="1" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.44140625" customWidth="1"/>
     <col min="10" max="10" width="18.88671875" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" customWidth="1"/>
     <col min="18" max="18" width="15.109375" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
@@ -33069,58 +33216,58 @@
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
         <v>14</v>
       </c>
@@ -33128,56 +33275,56 @@
         <v>7</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H3" s="35"/>
       <c r="J3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="R3" s="35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
         <v>18</v>
       </c>
@@ -33185,53 +33332,53 @@
         <v>7</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H4" s="35"/>
       <c r="J4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>22</v>
       </c>
@@ -33239,187 +33386,296 @@
         <v>7</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P5" s="35" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="Q5" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P6" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="M7" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="Q6" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1">
+      <c r="N7" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q7" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>160</v>
+        <v>171</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>171</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="N9" s="43" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+      <c r="N9" s="44" t="s">
+        <v>174</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P9" s="35" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="Q9" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R9" s="35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="S9" s="35" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="T9" s="35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A10" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A11" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q11" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" s="39" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A10" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:20" ht="15.75" customHeight="1"/>
+      <c r="S11" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -34403,6 +34659,9 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -34412,25 +34671,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="22.5546875" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" customWidth="1"/>
     <col min="19" max="19" width="16.88671875" customWidth="1"/>
-    <col min="20" max="20" width="28.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
+    <col min="20" max="20" width="28.33203125" customWidth="1"/>
+    <col min="21" max="21" width="19.77734375" customWidth="1"/>
     <col min="22" max="22" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -34439,67 +34696,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>175</v>
+        <v>190</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -34507,135 +34764,129 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="N2" s="35" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="P2" s="35" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R2" s="35">
         <v>400</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="37" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R3" s="35">
         <v>400</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -34643,67 +34894,191 @@
         <v>22</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K4" s="39" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="L4" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M4" s="39" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="O4" s="39" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="P4" s="39" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="39" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R4" s="41">
         <v>600</v>
       </c>
       <c r="S4" s="39" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="T4" s="39" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="R5" s="35">
+        <v>17800</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q6" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="R6" s="35">
+        <v>2000</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="U6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="V6" s="39" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -34720,66 +35095,63 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1"/>
     <col min="6" max="6" width="65.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="258" customHeight="1">
-      <c r="A2" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>198</v>
+      <c r="B1" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="172.5" customHeight="1">
+      <c r="A2" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>200</v>
+        <v>222</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>223</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="100.5" customHeight="1">
       <c r="A3" s="35" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>198</v>
+        <v>43</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -34799,7 +35171,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34814,10 +35186,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" customWidth="1"/>
     <col min="12" max="12" width="9.109375" customWidth="1"/>
     <col min="24" max="24" width="23.44140625" customWidth="1"/>
   </cols>
@@ -34827,147 +35199,147 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="44" t="s">
-        <v>207</v>
+        <v>109</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>229</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>175</v>
+        <v>190</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="K2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="S2" s="39" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="T2" s="41">
         <v>500</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="V2" s="39" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="W2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="X2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and Fixed the Extra fields in BT Payment Instrument according to new UI Changes under Account tab in Party
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -28,14 +28,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mjKYysnXdYZMAChtG/E4cS+Ia3avA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mhFMMTuNg2V55ynXonvWbOvDvhTMw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="334">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -840,9 +840,9 @@
   <si>
     <t>{
         "party": {
-                "dealRefId": "REF1678428748624",
-                "name": "Party7887",
-                "partyRefId": "Party7887",
+                "dealRefId": "REF1678956865900",
+                "name": "Party788791",
+                "partyRefId": "Party788791",
                 "country": "IN",
                 "status": "Active",
                 "kycCompleted": true,
@@ -30413,6 +30413,8 @@
     <col customWidth="1" min="2" max="2" width="13.88"/>
     <col customWidth="1" min="8" max="8" width="22.63"/>
     <col customWidth="1" min="10" max="10" width="19.75"/>
+    <col customWidth="1" min="12" max="12" width="21.0"/>
+    <col customWidth="1" min="13" max="13" width="28.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -30447,30 +30449,36 @@
         <v>140</v>
       </c>
       <c r="K1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="P1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>268</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>269</v>
       </c>
     </row>
@@ -30505,31 +30513,37 @@
       <c r="J2" s="34" t="s">
         <v>306</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="34">
+        <v>600.0</v>
+      </c>
+      <c r="L2" s="34" t="s">
         <v>157</v>
-      </c>
-      <c r="L2" s="34" t="s">
-        <v>158</v>
       </c>
       <c r="M2" s="34" t="s">
         <v>105</v>
       </c>
       <c r="N2" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="Q2" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="R2" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="R2" s="34" t="s">
+      <c r="T2" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="U2" s="34" t="s">
         <v>308</v>
       </c>
     </row>
@@ -33719,7 +33733,9 @@
       <c r="N2" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="O2" s="34"/>
+      <c r="O2" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="P2" s="34" t="s">
         <v>105</v>
       </c>
@@ -33780,7 +33796,9 @@
       <c r="N3" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="O3" s="34"/>
+      <c r="O3" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="P3" s="34" t="s">
         <v>109</v>
       </c>
@@ -33845,7 +33863,9 @@
       <c r="N4" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="O4" s="34"/>
+      <c r="O4" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="P4" s="34" t="s">
         <v>109</v>
       </c>
@@ -33912,7 +33932,9 @@
       <c r="N5" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="O5" s="34"/>
+      <c r="O5" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="P5" s="34" t="s">
         <v>105</v>
       </c>
@@ -33972,7 +33994,9 @@
       <c r="N6" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="O6" s="34"/>
+      <c r="O6" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="P6" s="34" t="s">
         <v>109</v>
       </c>
@@ -34038,7 +34062,9 @@
       <c r="N7" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="O7" s="38"/>
+      <c r="O7" s="38" t="s">
+        <v>105</v>
+      </c>
       <c r="P7" s="38" t="s">
         <v>105</v>
       </c>
@@ -34068,9 +34094,6 @@
       <c r="A8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="T8" s="34">
-        <v>600.0</v>
-      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="24" t="s">
@@ -34109,7 +34132,9 @@
       <c r="N9" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="O9" s="34"/>
+      <c r="O9" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="P9" s="34" t="s">
         <v>105</v>
       </c>
@@ -34178,7 +34203,9 @@
       <c r="N10" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="O10" s="34"/>
+      <c r="O10" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="P10" s="34" t="s">
         <v>105</v>
       </c>
@@ -34238,7 +34265,9 @@
       <c r="N11" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="O11" s="34"/>
+      <c r="O11" s="34" t="s">
+        <v>105</v>
+      </c>
       <c r="P11" s="34" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Updated excel sheet according to TS 13
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\dev\upp-test-automation\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -34,16 +29,17 @@
     <sheet name="Payment Profile" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:H15"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mhTAQv+vpR89b+9ZFSfU2Yp2bBa1g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mjKYysnXdYZMAChtG/E4cS+Ia3avA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="334">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -226,14 +222,14 @@
     <t>TS12</t>
   </si>
   <si>
-    <t xml:space="preserve">Create a Transaction in Transaction Maker , Transaction to
+    <t xml:space="preserve">Create a Transaction in Transaction Maker , with Transaction to
  Non Registered Beneficiary Checkbox  Unckecked in Basic Details Page in Deal </t>
   </si>
   <si>
     <t>TS13</t>
   </si>
   <si>
-    <t xml:space="preserve">Create a Transaction in Transaction Maker , Transaction to
+    <t xml:space="preserve">Create a Transaction in Transaction Maker , with Transaction to
  Non Registered Beneficiary Checkbox  Checked in Basic Details Page in Deal </t>
   </si>
   <si>
@@ -518,10 +514,25 @@
     <t>Beneficiary Bank Bic</t>
   </si>
   <si>
+    <t>Beneficiary Country Of Incorporation</t>
+  </si>
+  <si>
     <t>Beneficiary Country</t>
   </si>
   <si>
+    <t>werwer</t>
+  </si>
+  <si>
+    <t>Trteo</t>
+  </si>
+  <si>
     <t>To</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>accountType</t>
   </si>
   <si>
     <t>Beneficiary Currency</t>
@@ -570,6 +581,12 @@
   </si>
   <si>
     <t>BIC456</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>XYZTS12</t>
   </si>
   <si>
     <t>DIB4567</t>
@@ -659,6 +676,45 @@
     <t>IMDTS11</t>
   </si>
   <si>
+    <t>TestUser12</t>
+  </si>
+  <si>
+    <t>Test12 remarks</t>
+  </si>
+  <si>
+    <t>Testuser12@gmail.com</t>
+  </si>
+  <si>
+    <t>LTTest</t>
+  </si>
+  <si>
+    <t>SBITS12</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>TestUser13</t>
+  </si>
+  <si>
+    <t>Test13 remarks</t>
+  </si>
+  <si>
+    <t>Testuser13@gmail.com</t>
+  </si>
+  <si>
+    <t>ABC111</t>
+  </si>
+  <si>
+    <t>XYZTS13</t>
+  </si>
+  <si>
+    <t>SBITS13</t>
+  </si>
+  <si>
+    <t>OverDraft</t>
+  </si>
+  <si>
     <t>Select Instruction Type</t>
   </si>
   <si>
@@ -700,12 +756,6 @@
   </si>
   <si>
     <t>to</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Beneficiary Country Of Incorporation</t>
   </si>
   <si>
     <t>Retry-Enable Auto Retry</t>
@@ -794,9 +844,9 @@
   <si>
     <t>{
         "party": {
-                "dealRefId": "REF1678428748624",
-                "name": "Party1234567809",
-                "partyRefId": "Party1234567009",
+                "dealRefId": "REF1678956865900",
+                "name": "Party7887901",
+                "partyRefId": "Party7887901",
                 "country": "IN",
                 "status": "Active",
                 "kycCompleted": true,
@@ -837,9 +887,6 @@
                         "paymentInstrumentId": "BT",
                         "description": "Payout Account",
                         "paymentDetails": {
-                        "beneficiaryBankBic": "BIC456",
-                        "beneficiaryCountry":"IN",
-                        "beneficiaryCurrency":"INR",
                         "to":"SBI98765",
                         "beneficiaryCountryOfIncorporation":"IN",
                         "amount":1000
@@ -886,15 +933,6 @@
     <t>Sub Instruction - Instrument</t>
   </si>
   <si>
-    <t>werwer</t>
-  </si>
-  <si>
-    <t>Trteo</t>
-  </si>
-  <si>
-    <t>accountType</t>
-  </si>
-  <si>
     <t>beneficiaryCountry</t>
   </si>
   <si>
@@ -937,18 +975,6 @@
     <t>Adhoc Payment TS12</t>
   </si>
   <si>
-    <t>LTTest</t>
-  </si>
-  <si>
-    <t>ABC123</t>
-  </si>
-  <si>
-    <t>XYZTS12</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
     <t>https://sit.upp.appveen.com/</t>
   </si>
   <si>
@@ -956,18 +982,6 @@
   </si>
   <si>
     <t>Adhoc Payment TS13</t>
-  </si>
-  <si>
-    <t>SBITS13</t>
-  </si>
-  <si>
-    <t>ABC111</t>
-  </si>
-  <si>
-    <t>XYZTS13</t>
-  </si>
-  <si>
-    <t>OverDraft</t>
   </si>
   <si>
     <t>Test data TS13</t>
@@ -1009,7 +1023,13 @@
     <t>Fragment Platform Reference No</t>
   </si>
   <si>
+    <t>Instrument - category</t>
+  </si>
+  <si>
     <t>PartyABCD</t>
+  </si>
+  <si>
+    <t>Adhoc Payment1</t>
   </si>
   <si>
     <t>Creditorpartyid123</t>
@@ -1122,21 +1142,6 @@
   <si>
     <t>TT</t>
   </si>
-  <si>
-    <t>Test7 remarks</t>
-  </si>
-  <si>
-    <t>Instrument category</t>
-  </si>
-  <si>
-    <t>TestUser13</t>
-  </si>
-  <si>
-    <t>Test13 remarks</t>
-  </si>
-  <si>
-    <t>Testuser13@gmail.com</t>
-  </si>
 </sst>
 </file>
 
@@ -1146,7 +1151,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1230,13 +1235,6 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1295,11 +1293,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1387,14 +1384,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1403,10 +1400,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1626,8 +1621,8 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -29651,13 +29646,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>114</v>
@@ -29666,49 +29661,49 @@
         <v>111</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q1" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="R1" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="H1" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>246</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>247</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q1" s="44" t="s">
-        <v>251</v>
-      </c>
-      <c r="R1" s="34" t="s">
-        <v>227</v>
-      </c>
       <c r="S1" s="34" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="U1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -29716,16 +29711,16 @@
         <v>28</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>120</v>
@@ -29734,13 +29729,13 @@
         <v>84</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="K2" s="34">
         <v>500</v>
@@ -29753,19 +29748,19 @@
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
       <c r="Q2" s="34" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="R2" s="49" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="U2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -29773,55 +29768,58 @@
         <v>46</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>84</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>264</v>
+        <v>200</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>201</v>
       </c>
       <c r="L3" s="34" t="s">
         <v>105</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>265</v>
+        <v>166</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>266</v>
+        <v>167</v>
       </c>
       <c r="O3" s="34" t="s">
-        <v>267</v>
+        <v>202</v>
       </c>
       <c r="P3" s="34" t="s">
         <v>105</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="R3" s="49" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="S3" s="34" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="U3" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -29829,58 +29827,58 @@
         <v>48</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>84</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>264</v>
+        <v>200</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>271</v>
+        <v>208</v>
       </c>
       <c r="L4" s="34" t="s">
         <v>105</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>272</v>
+        <v>206</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>273</v>
+        <v>207</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>274</v>
+        <v>209</v>
       </c>
       <c r="P4" s="34" t="s">
         <v>105</v>
       </c>
       <c r="Q4" s="34" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="R4" s="49" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="S4" s="34" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="T4" s="34" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="U4" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -29914,13 +29912,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -29928,13 +29926,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -29942,13 +29940,13 @@
         <v>46</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -29956,13 +29954,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -29991,13 +29989,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30005,13 +30003,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -30019,13 +30017,13 @@
         <v>46</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30033,13 +30031,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -30069,9 +30067,7 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30096,67 +30092,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>136</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>114</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>287</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>326</v>
+        <v>293</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="P1" s="34" t="s">
         <v>142</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S1" s="44" t="s">
-        <v>251</v>
+        <v>143</v>
+      </c>
+      <c r="S1" s="41" t="s">
+        <v>266</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="U1" s="34" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -30164,25 +30160,25 @@
         <v>30</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>208</v>
+        <v>297</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>120</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>105</v>
@@ -30191,22 +30187,22 @@
         <v>104</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="O2" s="34" t="s">
         <v>70</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="Q2" s="34">
         <v>250</v>
@@ -30215,21 +30211,20 @@
         <v>105</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="U2" s="34" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="V2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30254,13 +30249,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30268,13 +30263,13 @@
         <v>30</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -30298,13 +30293,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30312,13 +30307,13 @@
         <v>30</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -30381,25 +30376,25 @@
         <v>142</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1">
@@ -30410,55 +30405,55 @@
         <v>7</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>67</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>68</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="M2" s="34" t="s">
         <v>105</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="O2" s="34" t="s">
         <v>104</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="R2" s="34" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -30486,10 +30481,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -30497,10 +30492,10 @@
         <v>34</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -30519,6 +30514,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" customWidth="1"/>
     <col min="11" max="11" width="26.33203125" customWidth="1"/>
@@ -30529,46 +30525,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -30576,46 +30572,46 @@
         <v>37</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="K2" s="37">
         <v>44991</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30630,9 +30626,7 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -32131,16 +32125,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -32151,7 +32145,7 @@
         <v>105</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
@@ -32160,7 +32154,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1"/>
@@ -33172,9 +33166,9 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -33532,11 +33526,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V998"/>
+  <dimension ref="A1:AA998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -33547,12 +33539,14 @@
     <col min="12" max="12" width="18.33203125" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" customWidth="1"/>
+    <col min="16" max="16" width="15.77734375" customWidth="1"/>
+    <col min="22" max="22" width="16.44140625" customWidth="1"/>
+    <col min="23" max="23" width="15.109375" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" customHeight="1">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -33595,16 +33589,16 @@
       <c r="N1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="41" t="s">
         <v>143</v>
       </c>
       <c r="P1" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="41" t="s">
         <v>146</v>
       </c>
       <c r="S1" s="34" t="s">
@@ -33613,8 +33607,23 @@
       <c r="T1" s="34" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1">
+      <c r="U1" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="X1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
@@ -33622,58 +33631,65 @@
         <v>7</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>68</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="O2" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q2" s="34" t="s">
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="T2" s="34">
+        <v>600</v>
+      </c>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="R2" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W2" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="X2" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
@@ -33681,56 +33697,67 @@
         <v>7</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>85</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>84</v>
       </c>
       <c r="H3" s="34"/>
       <c r="J3" s="34" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>84</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="O3" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="34" t="s">
-        <v>161</v>
-      </c>
       <c r="Q3" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="R3" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="T3" s="34">
+        <v>600</v>
+      </c>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="R3" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="S3" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="T3" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W3" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="X3" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y3" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="24" t="s">
         <v>18</v>
       </c>
@@ -33738,56 +33765,58 @@
         <v>7</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>325</v>
-      </c>
       <c r="G4" s="34" t="s">
         <v>84</v>
       </c>
       <c r="H4" s="34"/>
       <c r="J4" s="34" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="K4" s="34" t="s">
         <v>84</v>
       </c>
       <c r="L4" s="34" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N4" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="O4" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q4" s="34" t="s">
+      <c r="S4" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="T4" s="34">
+        <v>600</v>
+      </c>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="R4" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="S4" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="T4" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W4" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="X4" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y4" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="24" t="s">
         <v>22</v>
       </c>
@@ -33795,58 +33824,65 @@
         <v>7</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>69</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>68</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="I5" s="34" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="K5" s="34" t="s">
         <v>68</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N5" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="O5" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P5" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q5" s="34" t="s">
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="T5" s="34">
+        <v>600</v>
+      </c>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="R5" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="S5" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W5" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="X5" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="24" t="s">
         <v>28</v>
       </c>
@@ -33854,52 +33890,59 @@
         <v>7</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>85</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>84</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K6" s="34" t="s">
         <v>84</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N6" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="O6" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="34" t="s">
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="T6" s="34">
+        <v>600</v>
+      </c>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="W6" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="X6" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="Q6" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="R6" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="S6" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="24" t="s">
         <v>30</v>
       </c>
@@ -33907,66 +33950,76 @@
         <v>7</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G7" s="38" t="s">
         <v>68</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="K7" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="41" t="s">
-        <v>176</v>
+      <c r="L7" s="42" t="s">
+        <v>183</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N7" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="O7" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="P7" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q7" s="38" t="s">
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="T7" s="34">
+        <v>600</v>
+      </c>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="R7" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="S7" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W7" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="X7" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="32"/>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1">
+      <c r="T8" s="34">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="24" t="s">
         <v>34</v>
       </c>
@@ -33974,55 +34027,62 @@
         <v>7</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>177</v>
+        <v>184</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>184</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>95</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="G9" s="34" t="s">
         <v>84</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="K9" s="34" t="s">
         <v>68</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="N9" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="O9" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="N9" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="T9" s="34">
+        <v>600</v>
+      </c>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="R9" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="S9" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="T9" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W9" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="X9" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y9" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="24" t="s">
         <v>37</v>
       </c>
@@ -34030,58 +34090,65 @@
         <v>7</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>69</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G10" s="34" t="s">
         <v>84</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="I10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="K10" s="34" t="s">
         <v>68</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="O10" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P10" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q10" s="34" t="s">
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="T10" s="34">
+        <v>600</v>
+      </c>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="R10" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="S10" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1">
+      <c r="W10" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="X10" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="34" t="s">
         <v>43</v>
       </c>
@@ -34089,112 +34156,187 @@
         <v>7</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>185</v>
+        <v>192</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>192</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>85</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>84</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="K11" s="34" t="s">
         <v>84</v>
       </c>
       <c r="L11" s="34" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="N11" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="O11" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P11" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q11" s="34" t="s">
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="T11" s="34">
+        <v>600</v>
+      </c>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="R11" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="S11" s="38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A13" s="24" t="s">
+      <c r="W11" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="X11" s="38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A12" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="M12" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="N12" s="44"/>
+      <c r="O12" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="P12" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q12" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="T12" s="34">
+        <v>600</v>
+      </c>
+      <c r="U12" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="W12" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="X12" s="38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A13" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>327</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>327</v>
-      </c>
-      <c r="E13" s="47" t="s">
+      <c r="C13" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="47" t="s">
-        <v>328</v>
-      </c>
-      <c r="G13" s="47" t="s">
+      <c r="F13" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="47"/>
-      <c r="J13" s="47" t="s">
-        <v>327</v>
-      </c>
-      <c r="K13" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" s="51" t="s">
-        <v>329</v>
-      </c>
-      <c r="M13" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="N13" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="O13" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P13" s="47" t="s">
+      <c r="J13" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="N13" s="43"/>
+      <c r="O13" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="R13" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="T13" s="34">
+        <v>600</v>
+      </c>
+      <c r="U13" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="W13" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="X13" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="Q13" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="R13" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="S13" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="T13" s="47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -35180,7 +35322,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L7" r:id="rId1"/>
-    <hyperlink ref="L13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35216,10 +35357,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>114</v>
@@ -35228,55 +35369,55 @@
         <v>111</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>200</v>
+        <v>219</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>220</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="S1" s="34" t="s">
         <v>142</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="U1" s="34" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -35284,19 +35425,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>120</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>122</v>
@@ -35311,16 +35452,16 @@
         <v>122</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="Q2" s="34" t="s">
         <v>124</v>
@@ -35329,7 +35470,7 @@
         <v>400</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="T2" s="34" t="s">
         <v>109</v>
@@ -35343,22 +35484,22 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="36" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>120</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>122</v>
@@ -35373,19 +35514,19 @@
         <v>122</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="N3" s="34" t="s">
         <v>119</v>
       </c>
       <c r="O3" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="P3" s="34" t="s">
         <v>123</v>
@@ -35397,7 +35538,7 @@
         <v>400</v>
       </c>
       <c r="S3" s="34" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="T3" s="34" t="s">
         <v>109</v>
@@ -35414,19 +35555,19 @@
         <v>22</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>120</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="G4" s="38" t="s">
         <v>122</v>
@@ -35441,19 +35582,19 @@
         <v>122</v>
       </c>
       <c r="K4" s="38" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="L4" s="38" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="N4" s="38" t="s">
         <v>119</v>
       </c>
       <c r="O4" s="38" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="P4" s="38" t="s">
         <v>128</v>
@@ -35465,7 +35606,7 @@
         <v>600</v>
       </c>
       <c r="S4" s="38" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="T4" s="38" t="s">
         <v>109</v>
@@ -35482,19 +35623,19 @@
         <v>34</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>219</v>
+        <v>226</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>237</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>120</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>122</v>
@@ -35509,16 +35650,16 @@
         <v>122</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="Q5" s="38" t="s">
         <v>124</v>
@@ -35527,7 +35668,7 @@
         <v>17800</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="T5" s="34" t="s">
         <v>105</v>
@@ -35544,19 +35685,19 @@
         <v>37</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>120</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="G6" s="38" t="s">
         <v>122</v>
@@ -35571,19 +35712,19 @@
         <v>122</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="N6" s="38" t="s">
         <v>119</v>
       </c>
       <c r="O6" s="38" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="P6" s="38" t="s">
         <v>128</v>
@@ -35595,7 +35736,7 @@
         <v>500</v>
       </c>
       <c r="S6" s="38" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="T6" s="38" t="s">
         <v>105</v>
@@ -35612,19 +35753,19 @@
         <v>43</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>223</v>
+        <v>226</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>241</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>120</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="G7" s="38" t="s">
         <v>122</v>
@@ -35639,25 +35780,25 @@
         <v>122</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="M7" s="34" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="Q7" s="38" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="R7" s="34">
         <v>2000</v>
       </c>
       <c r="S7" s="34" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="T7" s="34" t="s">
         <v>105</v>
@@ -35696,50 +35837,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="172.5" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="100.5" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -35787,10 +35928,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>114</v>
@@ -35799,61 +35940,61 @@
         <v>111</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="44" t="s">
-        <v>238</v>
+      <c r="K1" s="41" t="s">
+        <v>256</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>200</v>
+        <v>219</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>220</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="R1" s="34" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="U1" s="34" t="s">
         <v>142</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -35861,19 +36002,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>120</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="G2" s="38" t="s">
         <v>122</v>
@@ -35882,10 +36023,10 @@
         <v>122</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="K2" s="38" t="s">
         <v>7</v>
@@ -35894,19 +36035,19 @@
         <v>122</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="P2" s="38" t="s">
         <v>65</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="R2" s="38" t="s">
         <v>65</v>
@@ -35918,7 +36059,7 @@
         <v>500</v>
       </c>
       <c r="U2" s="38" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="V2" s="38" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
TS05 modified and TS10 added
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\upp-test-automation\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3975" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -29,17 +34,16 @@
     <sheet name="Payment Profile" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H15"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7mgG4Sl0IX8+8z1LblT6PwhF9HRwcA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId24" roundtripDataSignature="AMtx7miH7zaeOoXaO+HROu0JwChLWuaB/Q=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="305">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -141,6 +145,9 @@
     <t>TS05-Assertion</t>
   </si>
   <si>
+    <t>Assertion for Budget details</t>
+  </si>
+  <si>
     <t>In the Budget Screen, validate the Available Budget and Utilized budget next day</t>
   </si>
   <si>
@@ -192,14 +199,28 @@
     <t>a) Creating a Holiday for Future date (Ex: 06-March-2023) and [TS03] creating a SCHD txn for the same date and because of holiday Action(next business day), txn should be schd for 07-March-2023 and executed on the same date</t>
   </si>
   <si>
-    <t>TS03-assertion1</t>
+    <t>TS10-assertion1</t>
   </si>
   <si>
-    <t>TS10- Assertion for TS 10</t>
+    <t>Assertion for TS 10</t>
   </si>
   <si>
     <t>As per the Holiday Configuration and Holiday action, transaction should be created and executed accordingly.
 Note: Validate the txn schd date</t>
+  </si>
+  <si>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>Basic Details
+Accounts
+Party
+Payments
+(AND)
+PARTY API</t>
+  </si>
+  <si>
+    <t>TS03 + Add Party through Api and creating a txn</t>
   </si>
   <si>
     <t>Deal Name</t>
@@ -319,7 +340,13 @@
     <t>TS05_Deal</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>TS06_Deal</t>
+  </si>
+  <si>
+    <t>TS07_Deal</t>
   </si>
   <si>
     <t>TS09_Deal</t>
@@ -332,6 +359,15 @@
   </si>
   <si>
     <t>Acquirer</t>
+  </si>
+  <si>
+    <t>TS10_Deal_Holiday</t>
+  </si>
+  <si>
+    <t>TS011_Deal</t>
+  </si>
+  <si>
+    <t>ALL</t>
   </si>
   <si>
     <t>Currency</t>
@@ -558,6 +594,12 @@
     <t>BICTS06</t>
   </si>
   <si>
+    <t>TestUser7</t>
+  </si>
+  <si>
+    <t>Testuser7@gmail.com</t>
+  </si>
+  <si>
     <t>TestUser9</t>
   </si>
   <si>
@@ -571,6 +613,30 @@
   </si>
   <si>
     <t>IMDTS09</t>
+  </si>
+  <si>
+    <t>TestUser10</t>
+  </si>
+  <si>
+    <t>Test10 remarks</t>
+  </si>
+  <si>
+    <t>Testuser10@gmail.com</t>
+  </si>
+  <si>
+    <t>TestUser11</t>
+  </si>
+  <si>
+    <t>Test11 remarks</t>
+  </si>
+  <si>
+    <t>Testuser11@gmail.com</t>
+  </si>
+  <si>
+    <t>BICTS11</t>
+  </si>
+  <si>
+    <t>IMDTS11</t>
   </si>
   <si>
     <t>Select Instruction Type</t>
@@ -646,6 +712,9 @@
     <t>SCBASDFGH</t>
   </si>
   <si>
+    <t>TS03-assertion1</t>
+  </si>
+  <si>
     <t>March 06-2023</t>
   </si>
   <si>
@@ -655,10 +724,31 @@
     <t>Bill</t>
   </si>
   <si>
+    <t>At specific time</t>
+  </si>
+  <si>
+    <t>Bill Payment</t>
+  </si>
+  <si>
+    <t>Ledger Balance</t>
+  </si>
+  <si>
+    <t>Do not execute on holiday</t>
+  </si>
+  <si>
+    <t>ICICI178</t>
+  </si>
+  <si>
+    <t>TS11 Payment</t>
+  </si>
+  <si>
+    <t>SBITS11</t>
+  </si>
+  <si>
     <t>Parent Test case</t>
   </si>
   <si>
-    <t>PArty Type</t>
+    <t>Party Type</t>
   </si>
   <si>
     <t>URL</t>
@@ -667,16 +757,13 @@
     <t>Method</t>
   </si>
   <si>
-    <t>PAyload</t>
+    <t>Payload</t>
   </si>
   <si>
-    <t>TS12-1</t>
+    <t>TS11-1</t>
   </si>
   <si>
-    <t>TS12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Individual</t>
+    <t>Company</t>
   </si>
   <si>
     <t>https://dev.upp.appveen.com/mdm/api/party</t>
@@ -687,19 +774,15 @@
   <si>
     <t>{
         "party": {
-                "dealRefId": "REF1672297910549",
-                "name": "Ranjith123",
-                "partyRefId": "Ranjith123",
+                "dealRefId": "REF1678428748624",
+                "name": "Party1234567809",
+                "partyRefId": "Party1234567009",
                 "country": "IN",
                 "status": "Active",
                 "kycCompleted": true,
                 "validFrom": "2021-09-17",
                 "validUntil": "2023-12-31",
                 "responsibility": "Acquiree",
-                "attributes": {
-                        "acquiree": "Merchant",
-                        "number": 10
-                },
 "type":"company",
 "company":{
 "incorporationDate":"2021-09-17",
@@ -731,108 +814,25 @@
                         }
                 }],
                 "accounts": [{
-                        "paymentInstrumentId": "AK-Pay",
+                        "paymentInstrumentId": "BT",
                         "description": "Payout Account",
                         "paymentDetails": {
-                                "accountIban": "Account Number",
-                                "to": "123123122133",
-                                "receiverPop": "123",
-                                "name": "Merchant293",
-                                "beneficiaryCountry": "IN",
-                                "beneficiaryCurrency": "INR"
-                        },
-            "overrides": [{
-                    "profileName": "Payment Profile",
-                    "paymentInstrument":"BT",
-                    "country": "IN",
-                    "attributes": [
-                        {
-                            "name": "Charge Bearer",
-                            "value": "SHA"
+                        "beneficiaryBankBic": "BIC456",
+                        "beneficiaryCountry":"IN",
+                        "beneficiaryCurrency":"INR",
+                        "to":"SBI98765",
+                        "beneficiaryCountryOfIncorporation":"IN",
+                        "amount":1000
                         }
-                    ]
-                }]
                 }]
         }
 }</t>
   </si>
   <si>
-    <t>TS12-2</t>
+    <t>TS11-2</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>{
-        "party": {
-                "dealRefId": "REF1672297910549",
-                "name": "Karthik123",
-                "partyRefId": "Karthik123",
-                "country": "IN",
-                "status": "Active",
-                "kycCompleted": true,
-                "validFrom": "2021-09-17",
-                "validUntil": "2023-12-31",
-                "responsibility": "Acquiree",
-                "attributes": {
-                        "acquiree": "Merchant",
-                        "number": 10
-                },
-"type":"company",
-"company":{
-"incorporationDate":"2021-09-17",
-"registrationNumber":"REG123432",
-"taxId":"",
-"taxType":"",
-"businessCategory":"",
-"businessType":"",
-"listingAuthority":""
-},
-                "executionPolicies": {
-                        "onPartyActivate": "doNothing",
-                        "onPartyDeactivate": "holdExecutions"
-                },
-                "contacts": [{
-                        "name": "Merchant33",
-                        "designation": "Manager",
-                        "authorizedSignatory": false,
-                        "enableNotifications": false,
-                        "workPhone": "+91 92392 29932",
-                        "mobilePhone": "+91 92392 29932",
-                        "email": "jane.doe@gmail.com",
-                        "address": {
-                                "town": "Bengaluru Urban",
-                                "street": "M G Road",
-                                "zip_pin": "4000340",
-                                "state": "KA",
-                                "country": "IN"
-                        }
-                }],
-                "accounts": [{
-                        "paymentInstrumentId": "AK-Pay",
-                        "description": "Payout Account",
-                        "paymentDetails": {
-                                "accountIban": "Account Number",
-                                "to": "123123122133",
-                                "receiverPop": "123",
-                                "name": "Merchant293",
-                                "beneficiaryCountry": "IN",
-                                "beneficiaryCurrency": "INR"
-                        },
-            "overrides": [{
-                    "profileName": "Payment Profile",
-                    "paymentInstrument":"BT",
-                    "country": "IN",
-                    "attributes": [
-                        {
-                            "name": "Charge Bearer",
-                            "value": "SHA"
-                        }
-                    ]
-                }]
-                }]
-        }
-}</t>
+    <t>Individual</t>
   </si>
   <si>
     <t>Linked - Amount</t>
@@ -849,9 +849,6 @@
   </si>
   <si>
     <t>Disabled</t>
-  </si>
-  <si>
-    <t>At specific time</t>
   </si>
   <si>
     <t>CREATE TRANSACTION - Deal Ref Id</t>
@@ -974,7 +971,7 @@
     <t>Should be same as Ecomm Maker screen amount</t>
   </si>
   <si>
-    <t>TestUser100</t>
+    <t>TestUser1002</t>
   </si>
   <si>
     <t>Testuser100@gmail.com</t>
@@ -1031,9 +1028,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Creating a new holiday for March 06</t>
-  </si>
-  <si>
     <t>Test Description</t>
   </si>
   <si>
@@ -1064,18 +1058,18 @@
     <t>TT</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>TS10 Holiday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1128,6 +1122,25 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1201,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1247,9 +1260,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1290,6 +1305,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1297,8 +1313,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1524,14 +1546,14 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -1770,10 +1792,14 @@
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="3"/>
@@ -1799,14 +1825,14 @@
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="11" t="s">
@@ -1835,18 +1861,18 @@
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1871,14 +1897,14 @@
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="11" t="s">
@@ -1907,16 +1933,16 @@
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="11" t="s">
@@ -1945,16 +1971,16 @@
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="9"/>
@@ -1978,22 +2004,24 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:26" ht="68.25" customHeight="1">
+      <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18" t="s">
-        <v>40</v>
+      <c r="D13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -2015,15 +2043,23 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -2045,13 +2081,13 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -2073,13 +2109,13 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -29498,15 +29534,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="7" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -29514,105 +29550,105 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>217</v>
+        <v>198</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>241</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="K2" s="35">
         <v>500</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="N2" s="45" t="s">
-        <v>225</v>
+        <v>248</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>249</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -29632,11 +29668,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29644,27 +29680,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -29681,11 +29717,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29693,27 +29729,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -29730,7 +29766,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29745,22 +29781,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="23.109375" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" customWidth="1"/>
-    <col min="15" max="16" width="23.109375" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" customWidth="1"/>
-    <col min="18" max="18" width="23.109375" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="16" width="23.140625" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -29768,135 +29804,135 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="N1" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="S1" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="P1" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="S1" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>218</v>
-      </c>
       <c r="U1" s="35" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="Q2" s="35">
         <v>250</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -29913,11 +29949,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29925,27 +29961,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -29962,34 +29998,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -30006,12 +30042,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1">
@@ -30019,117 +30055,117 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>59</v>
+        <v>144</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>63</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -30146,10 +30182,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -30157,21 +30193,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -30186,13 +30222,15 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -30200,93 +30238,93 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>271</v>
+        <v>304</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="K2" s="38">
         <v>44991</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -30301,21 +30339,19 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="10" width="16.88671875" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -30323,40 +30359,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -30364,40 +30400,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C2" s="22">
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -30405,30 +30441,30 @@
         <v>10</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L3" s="27"/>
     </row>
@@ -30437,34 +30473,34 @@
         <v>14</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C4" s="26">
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L4" s="27"/>
     </row>
@@ -30473,34 +30509,34 @@
         <v>18</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C5" s="30">
         <v>1</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L5" s="32"/>
       <c r="M5" s="33"/>
@@ -30510,121 +30546,214 @@
         <v>22</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>281</v>
+        <v>84</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>85</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C7" s="35">
         <v>1</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C10" s="35">
         <v>1</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J10" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1"/>
+      <c r="D11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="14" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="15" spans="1:13" ht="15.75" customHeight="1"/>
@@ -31627,13 +31756,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="1" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -31641,16 +31770,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -31658,19 +31787,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1"/>
@@ -32680,17 +32809,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -32698,16 +32827,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -32715,16 +32844,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -32732,16 +32861,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -32749,16 +32878,16 @@
         <v>14</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -32766,16 +32895,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -32783,65 +32912,94 @@
         <v>22</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -32858,13 +33016,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -32872,37 +33030,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -32910,28 +33068,28 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="J2" s="35">
         <v>1000</v>
@@ -32948,17 +33106,17 @@
         <v>22</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="39" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I3" s="40">
         <v>45130</v>
@@ -32979,89 +33137,87 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T998"/>
+  <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="1" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
@@ -33069,58 +33225,58 @@
         <v>7</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
         <v>14</v>
       </c>
@@ -33128,56 +33284,56 @@
         <v>7</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H3" s="35"/>
       <c r="J3" s="35" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="R3" s="35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
         <v>18</v>
       </c>
@@ -33185,53 +33341,53 @@
         <v>7</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H4" s="35"/>
       <c r="J4" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>22</v>
       </c>
@@ -33239,187 +33395,350 @@
         <v>7</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P5" s="35" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="Q5" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="P6" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="M7" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="Q6" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1">
+      <c r="N7" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q7" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>160</v>
+        <v>171</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>171</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="N9" s="43" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+      <c r="N9" s="44" t="s">
+        <v>174</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="P9" s="35" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="Q9" s="35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="R9" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="S9" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="T9" s="35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A10" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N10" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="S9" s="35" t="s">
+      <c r="O10" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="P10" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="T9" s="35" t="s">
+      <c r="Q10" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="R10" s="35" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A10" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:20" ht="15.75" customHeight="1"/>
+      <c r="S10" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A11" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q11" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="S11" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -34403,6 +34722,9 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -34412,26 +34734,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="22.5546875" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
-    <col min="20" max="20" width="28.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
-    <col min="22" max="22" width="23.109375" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
+    <col min="20" max="20" width="28.42578125" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" customWidth="1"/>
+    <col min="22" max="22" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -34439,67 +34759,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>175</v>
+        <v>193</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>194</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -34507,135 +34827,129 @@
         <v>14</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="N2" s="35" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="P2" s="35" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R2" s="35">
         <v>400</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="37" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R3" s="35">
         <v>400</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V3" s="35" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -34643,67 +34957,259 @@
         <v>22</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K4" s="39" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="L4" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M4" s="39" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="O4" s="39" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="P4" s="39" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="39" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R4" s="41">
         <v>600</v>
       </c>
       <c r="S4" s="39" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="T4" s="39" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="U4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="V4" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="R5" s="35">
+        <v>17800</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="N6" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" s="41">
+        <v>500</v>
+      </c>
+      <c r="S6" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="T6" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="U6" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="V6" s="39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="O7" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q7" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="R7" s="35">
+        <v>2000</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="U7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="V7" s="39" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -34720,66 +35226,63 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" customWidth="1"/>
-    <col min="6" max="6" width="65.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="12.75">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="258" customHeight="1">
-      <c r="A2" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>198</v>
+      <c r="B1" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="172.5" customHeight="1">
+      <c r="A2" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>200</v>
+        <v>225</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="100.5" customHeight="1">
       <c r="A3" s="35" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>198</v>
+        <v>43</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -34799,7 +35302,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34814,12 +35317,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
-    <col min="24" max="24" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -34827,147 +35330,147 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="44" t="s">
-        <v>207</v>
+        <v>109</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>232</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>175</v>
+        <v>193</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>194</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="K2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="S2" s="39" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="T2" s="41">
         <v>500</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="V2" s="39" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="W2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="X2" s="39" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed TS 13 - Updated TS04 - Updated TS07
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9084" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="7296" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="387">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -677,13 +677,7 @@
     <t>Deal_TS4</t>
   </si>
   <si>
-    <t>HDFC004</t>
-  </si>
-  <si>
     <t>Pune</t>
-  </si>
-  <si>
-    <t>BIC678</t>
   </si>
   <si>
     <t>TestUser5</t>
@@ -1195,9 +1189,6 @@
     <t>PartyABCD</t>
   </si>
   <si>
-    <t>Adhoc Payment1</t>
-  </si>
-  <si>
     <t>Creditorpartyid123</t>
   </si>
   <si>
@@ -1316,6 +1307,9 @@
   </si>
   <si>
     <t>TT</t>
+  </si>
+  <si>
+    <t>BIC124</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1320,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1420,6 +1414,13 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1478,10 +1479,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1593,8 +1595,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -29862,8 +29866,8 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -29886,13 +29890,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>312</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>314</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>121</v>
@@ -29901,16 +29905,16 @@
         <v>118</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>160</v>
@@ -29940,22 +29944,22 @@
         <v>161</v>
       </c>
       <c r="T1" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="U1" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="V1" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="W1" s="51" t="s">
         <v>317</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="X1" s="51" t="s">
         <v>318</v>
       </c>
-      <c r="V1" s="51" t="s">
-        <v>297</v>
-      </c>
-      <c r="W1" s="51" t="s">
+      <c r="Y1" s="51" t="s">
         <v>319</v>
-      </c>
-      <c r="X1" s="51" t="s">
-        <v>320</v>
-      </c>
-      <c r="Y1" s="51" t="s">
-        <v>321</v>
       </c>
       <c r="Z1" s="51"/>
     </row>
@@ -29964,16 +29968,16 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>323</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>324</v>
-      </c>
       <c r="E2" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>127</v>
@@ -29982,7 +29986,7 @@
         <v>92</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>174</v>
@@ -29997,13 +30001,13 @@
         <v>170</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N2" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>208</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>210</v>
       </c>
       <c r="P2" s="37" t="s">
         <v>116</v>
@@ -30015,19 +30019,19 @@
         <v>116</v>
       </c>
       <c r="U2" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="V2" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="W2" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="V2" s="53" t="s">
+      <c r="X2" s="37" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>327</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>328</v>
-      </c>
-      <c r="Y2" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -30035,28 +30039,28 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>92</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K3" s="37">
         <v>500</v>
@@ -30065,13 +30069,13 @@
         <v>182</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O3" s="37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>112</v>
@@ -30083,25 +30087,25 @@
         <v>188</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="T3" s="37" t="s">
         <v>112</v>
       </c>
       <c r="U3" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="V3" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="V3" s="53" t="s">
-        <v>331</v>
-      </c>
-      <c r="W3" s="37" t="s">
+      <c r="X3" s="37" t="s">
+        <v>330</v>
+      </c>
+      <c r="Y3" s="37" t="s">
         <v>327</v>
-      </c>
-      <c r="X3" s="37" t="s">
-        <v>332</v>
-      </c>
-      <c r="Y3" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -30109,28 +30113,28 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>92</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K4" s="37">
         <v>500</v>
@@ -30139,43 +30143,43 @@
         <v>170</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N4" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>112</v>
       </c>
       <c r="Q4" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="R4" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="S4" s="37" t="s">
         <v>250</v>
-      </c>
-      <c r="R4" s="37" t="s">
-        <v>251</v>
-      </c>
-      <c r="S4" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="T4" s="37" t="s">
         <v>112</v>
       </c>
       <c r="U4" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="V4" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="W4" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="V4" s="53" t="s">
-        <v>331</v>
-      </c>
-      <c r="W4" s="37" t="s">
+      <c r="X4" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y4" s="37" t="s">
         <v>327</v>
-      </c>
-      <c r="X4" s="37" t="s">
-        <v>334</v>
-      </c>
-      <c r="Y4" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -30209,13 +30213,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30223,13 +30227,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -30237,13 +30241,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30251,13 +30255,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30286,13 +30290,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30300,13 +30304,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>339</v>
-      </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -30314,13 +30318,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>339</v>
-      </c>
       <c r="D3" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30328,13 +30332,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>339</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30364,7 +30368,9 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30389,46 +30395,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>143</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>121</v>
       </c>
       <c r="F1" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>315</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>317</v>
-      </c>
-      <c r="J1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>342</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="N1" s="45" t="s">
         <v>344</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>345</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>346</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>347</v>
       </c>
       <c r="P1" s="37" t="s">
         <v>154</v>
@@ -30440,16 +30446,16 @@
         <v>155</v>
       </c>
       <c r="S1" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="T1" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="U1" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="V1" s="37" t="s">
         <v>319</v>
-      </c>
-      <c r="U1" s="37" t="s">
-        <v>320</v>
-      </c>
-      <c r="V1" s="37" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -30457,25 +30463,25 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>348</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>324</v>
-      </c>
       <c r="E2" s="37" t="s">
-        <v>349</v>
+        <v>268</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>127</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>112</v>
@@ -30484,22 +30490,22 @@
         <v>111</v>
       </c>
       <c r="K2" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>350</v>
+      </c>
+      <c r="N2" s="37" t="s">
         <v>351</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>352</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>353</v>
-      </c>
-      <c r="N2" s="37" t="s">
-        <v>354</v>
       </c>
       <c r="O2" s="37" t="s">
         <v>78</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="Q2" s="37">
         <v>250</v>
@@ -30508,16 +30514,16 @@
         <v>112</v>
       </c>
       <c r="S2" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="T2" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="U2" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="V2" s="37" t="s">
         <v>327</v>
-      </c>
-      <c r="U2" s="37" t="s">
-        <v>328</v>
-      </c>
-      <c r="V2" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -30546,13 +30552,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30560,13 +30566,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30590,13 +30596,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30604,13 +30610,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>339</v>
-      </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -30715,10 +30721,10 @@
         <v>164</v>
       </c>
       <c r="Y1" s="37" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Z1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
@@ -30729,10 +30735,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>100</v>
@@ -30744,28 +30750,28 @@
         <v>75</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>76</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="K2" s="37">
         <v>600</v>
       </c>
       <c r="L2" s="46" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="M2" s="37" t="s">
         <v>170</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="P2" s="37" t="s">
         <v>173</v>
@@ -30783,7 +30789,7 @@
         <v>112</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="V2" s="37" t="s">
         <v>111</v>
@@ -30795,10 +30801,10 @@
         <v>177</v>
       </c>
       <c r="Y2" s="37" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Z2" s="37" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -30826,10 +30832,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -30837,10 +30843,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -30870,46 +30876,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="G1" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="I1" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>320</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>370</v>
-      </c>
-      <c r="J1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>373</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>374</v>
-      </c>
-      <c r="N1" s="37" t="s">
-        <v>375</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -30917,46 +30923,46 @@
         <v>41</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>75</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K2" s="40">
         <v>44991</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -32470,16 +32476,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>384</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -32490,7 +32496,7 @@
         <v>112</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
@@ -32499,7 +32505,7 @@
         <v>114</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1"/>
@@ -33513,7 +33519,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -33645,10 +33651,34 @@
       <c r="A8" s="38" t="s">
         <v>34</v>
       </c>
+      <c r="B8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="38" t="s">
         <v>36</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -33873,7 +33903,9 @@
   </sheetPr>
   <dimension ref="A1:AF998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -34158,79 +34190,83 @@
       <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="37" t="s">
+      <c r="E4" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="37"/>
-      <c r="J4" s="37" t="s">
+      <c r="G4" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="K4" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="37" t="s">
+      <c r="I4" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="P4" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q4" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="R4" s="37" t="s">
+      <c r="O4" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="R4" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="S4" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="T4" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="U4" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="X4" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y4" s="37">
+      <c r="S4" s="51" t="s">
+        <v>386</v>
+      </c>
+      <c r="T4" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="U4" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y4" s="51">
         <v>600</v>
       </c>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB4" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC4" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD4" s="37" t="s">
-        <v>191</v>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB4" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC4" s="51" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="15.75" customHeight="1">
@@ -34241,49 +34277,49 @@
         <v>9</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>76</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M5" s="46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N5" s="37" t="s">
         <v>182</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P5" s="37" t="s">
         <v>172</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R5" s="37" t="s">
         <v>174</v>
@@ -34324,49 +34360,49 @@
         <v>9</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>93</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G6" s="37" t="s">
         <v>92</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K6" s="37" t="s">
         <v>92</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N6" s="37" t="s">
         <v>170</v>
       </c>
       <c r="O6" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P6" s="37" t="s">
         <v>184</v>
       </c>
       <c r="Q6" s="37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R6" s="37" t="s">
         <v>174</v>
       </c>
       <c r="S6" s="37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="T6" s="37" t="s">
         <v>116</v>
@@ -34401,10 +34437,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>77</v>
@@ -34416,34 +34452,34 @@
         <v>76</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I7" s="41" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K7" s="41" t="s">
         <v>76</v>
       </c>
       <c r="L7" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M7" s="46" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N7" s="37" t="s">
         <v>182</v>
       </c>
       <c r="O7" s="37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P7" s="41" t="s">
         <v>172</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R7" s="37" t="s">
         <v>174</v>
@@ -34493,40 +34529,40 @@
         <v>9</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>102</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G9" s="37" t="s">
         <v>92</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M9" s="46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N9" s="37" t="s">
         <v>170</v>
       </c>
       <c r="O9" s="37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P9" s="37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q9" s="37" t="s">
         <v>173</v>
@@ -34535,7 +34571,7 @@
         <v>174</v>
       </c>
       <c r="S9" s="48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T9" s="37" t="s">
         <v>112</v>
@@ -34546,7 +34582,7 @@
       <c r="V9" s="37"/>
       <c r="W9" s="37"/>
       <c r="X9" s="37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Y9" s="37">
         <v>600</v>
@@ -34573,43 +34609,43 @@
         <v>9</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>77</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G10" s="37" t="s">
         <v>92</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K10" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L10" s="37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N10" s="37" t="s">
         <v>182</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P10" s="37" t="s">
         <v>172</v>
@@ -34656,49 +34692,49 @@
         <v>9</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>93</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>92</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K11" s="37" t="s">
         <v>92</v>
       </c>
       <c r="L11" s="37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M11" s="46" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N11" s="37" t="s">
         <v>170</v>
       </c>
       <c r="O11" s="37" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P11" s="37" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q11" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R11" s="37" t="s">
         <v>174</v>
       </c>
       <c r="S11" s="48" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="T11" s="37" t="s">
         <v>112</v>
@@ -34709,7 +34745,7 @@
       <c r="V11" s="37"/>
       <c r="W11" s="37"/>
       <c r="X11" s="37" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Y11" s="37">
         <v>600</v>
@@ -34733,46 +34769,46 @@
         <v>9</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>93</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G12" s="37" t="s">
         <v>92</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K12" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L12" s="37" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N12" s="37" t="s">
         <v>182</v>
       </c>
       <c r="O12" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q12" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="R12" s="37" t="s">
         <v>240</v>
-      </c>
-      <c r="P12" s="37" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q12" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="R12" s="37" t="s">
-        <v>242</v>
       </c>
       <c r="S12" s="48"/>
       <c r="T12" s="37" t="s">
@@ -34788,13 +34824,13 @@
         <v>188</v>
       </c>
       <c r="X12" s="37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Y12" s="37">
         <v>600</v>
       </c>
       <c r="Z12" s="37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AB12" s="41" t="s">
         <v>176</v>
@@ -34811,46 +34847,46 @@
         <v>9</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E13" s="37" t="s">
         <v>93</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G13" s="37" t="s">
         <v>92</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K13" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L13" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M13" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N13" s="37" t="s">
         <v>170</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="P13" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q13" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R13" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="S13" s="46"/>
       <c r="T13" s="37" t="s">
@@ -34860,19 +34896,19 @@
         <v>112</v>
       </c>
       <c r="V13" s="37" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="W13" s="37" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="X13" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Y13" s="37">
         <v>600</v>
       </c>
       <c r="Z13" s="37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AB13" s="41" t="s">
         <v>176</v>
@@ -35869,6 +35905,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L7" r:id="rId1"/>
+    <hyperlink ref="L4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35904,10 +35941,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>121</v>
@@ -35916,40 +35953,40 @@
         <v>118</v>
       </c>
       <c r="F1" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>258</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="N1" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="P1" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>264</v>
-      </c>
-      <c r="P1" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>266</v>
       </c>
       <c r="R1" s="37" t="s">
         <v>160</v>
@@ -35970,16 +36007,16 @@
         <v>149</v>
       </c>
       <c r="X1" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Y1" s="37" t="s">
         <v>155</v>
       </c>
       <c r="Z1" s="37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AA1" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -35987,19 +36024,19 @@
         <v>17</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G2" s="37" t="s">
         <v>129</v>
@@ -36017,13 +36054,13 @@
         <v>191</v>
       </c>
       <c r="L2" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>273</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>275</v>
       </c>
       <c r="Q2" s="37" t="s">
         <v>131</v>
@@ -36032,7 +36069,7 @@
         <v>400</v>
       </c>
       <c r="S2" s="37" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T2" s="37" t="s">
         <v>185</v>
@@ -36047,7 +36084,7 @@
         <v>182</v>
       </c>
       <c r="X2" s="37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Y2" s="37" t="s">
         <v>116</v>
@@ -36061,22 +36098,22 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>127</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>129</v>
@@ -36091,19 +36128,19 @@
         <v>129</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N3" s="37" t="s">
         <v>126</v>
       </c>
       <c r="O3" s="37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P3" s="37" t="s">
         <v>130</v>
@@ -36115,14 +36152,14 @@
         <v>400</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T3" s="37"/>
       <c r="U3" s="37"/>
       <c r="V3" s="37"/>
       <c r="W3" s="37"/>
       <c r="X3" s="37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Y3" s="37" t="s">
         <v>116</v>
@@ -36139,19 +36176,19 @@
         <v>25</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E4" s="41" t="s">
         <v>127</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G4" s="41" t="s">
         <v>129</v>
@@ -36169,16 +36206,16 @@
         <v>191</v>
       </c>
       <c r="L4" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M4" s="41" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N4" s="41" t="s">
         <v>126</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P4" s="41" t="s">
         <v>135</v>
@@ -36190,22 +36227,22 @@
         <v>600</v>
       </c>
       <c r="S4" s="41" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="V4" s="37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="W4" s="37" t="s">
         <v>182</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="Y4" s="41" t="s">
         <v>116</v>
@@ -36222,19 +36259,19 @@
         <v>38</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>127</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>129</v>
@@ -36252,10 +36289,10 @@
         <v>191</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O5" s="37" t="s">
         <v>174</v>
@@ -36267,22 +36304,22 @@
         <v>17800</v>
       </c>
       <c r="S5" s="37" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="T5" s="37" t="s">
         <v>173</v>
       </c>
       <c r="U5" s="37" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="V5" s="37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="W5" s="37" t="s">
         <v>170</v>
       </c>
       <c r="X5" s="37" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Y5" s="37" t="s">
         <v>112</v>
@@ -36299,19 +36336,19 @@
         <v>41</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E6" s="41" t="s">
         <v>127</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G6" s="41" t="s">
         <v>129</v>
@@ -36329,16 +36366,16 @@
         <v>191</v>
       </c>
       <c r="L6" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M6" s="41" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N6" s="41" t="s">
         <v>126</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P6" s="41" t="s">
         <v>135</v>
@@ -36350,22 +36387,22 @@
         <v>500</v>
       </c>
       <c r="S6" s="41" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T6" s="37" t="s">
         <v>185</v>
       </c>
       <c r="U6" s="37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="V6" s="37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="W6" s="37" t="s">
         <v>182</v>
       </c>
       <c r="X6" s="37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Y6" s="41" t="s">
         <v>112</v>
@@ -36382,19 +36419,19 @@
         <v>49</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>127</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>129</v>
@@ -36412,37 +36449,37 @@
         <v>191</v>
       </c>
       <c r="L7" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O7" s="37" t="s">
         <v>174</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="R7" s="37">
         <v>2000</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="T7" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="V7" s="37" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="W7" s="37" t="s">
         <v>170</v>
       </c>
       <c r="X7" s="37" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Y7" s="37" t="s">
         <v>112</v>
@@ -36481,50 +36518,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="50" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>297</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>298</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="172.5" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="F2" s="37" t="s">
         <v>302</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="100.5" customHeight="1">
       <c r="A3" s="37" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -36555,27 +36592,52 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.109375" customWidth="1"/>
-    <col min="24" max="24" width="23.44140625" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:27">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>121</v>
@@ -36584,81 +36646,90 @@
         <v>118</v>
       </c>
       <c r="F1" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>257</v>
-      </c>
       <c r="I1" s="37" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J1" s="37" t="s">
         <v>122</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M1" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="P1" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="R1" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="S1" s="37" t="s">
         <v>264</v>
-      </c>
-      <c r="R1" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>266</v>
       </c>
       <c r="T1" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="U1" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="V1" s="37" t="s">
+      <c r="U1" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="V1" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y1" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="W1" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="X1" s="37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Z1" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA1" s="37" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="54" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>129</v>
@@ -36667,10 +36738,10 @@
         <v>129</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J2" s="41" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K2" s="41" t="s">
         <v>9</v>
@@ -36682,16 +36753,16 @@
         <v>191</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="O2" s="41" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P2" s="41" t="s">
         <v>73</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>281</v>
+        <v>174</v>
       </c>
       <c r="R2" s="41" t="s">
         <v>73</v>
@@ -36702,16 +36773,25 @@
       <c r="T2" s="43">
         <v>500</v>
       </c>
-      <c r="U2" s="41" t="s">
-        <v>276</v>
-      </c>
-      <c r="V2" s="41" t="s">
+      <c r="U2" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="W2" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="X2" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y2" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="W2" s="41" t="s">
+      <c r="Z2" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="X2" s="41" t="s">
+      <c r="AA2" s="41" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TS10 and TS02 Updated
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3975" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3975" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Master" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="389">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>TS02_Deal</t>
-  </si>
-  <si>
-    <t>flexible funding</t>
   </si>
   <si>
     <t>Mumbai HO</t>
@@ -1285,9 +1282,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Creating a new holiday for March 06</t>
-  </si>
-  <si>
     <t>Test Description</t>
   </si>
   <si>
@@ -1319,6 +1313,9 @@
   </si>
   <si>
     <t>Next business day</t>
+  </si>
+  <si>
+    <t>TS-10 Holiday</t>
   </si>
 </sst>
 </file>
@@ -29887,76 +29884,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="T1" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="J1" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="R1" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="S1" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="T1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="V1" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="W1" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="V1" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="W1" s="37" t="s">
+      <c r="X1" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="Y1" s="37" t="s">
         <v>320</v>
-      </c>
-      <c r="Y1" s="37" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -29964,70 +29961,70 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>324</v>
-      </c>
       <c r="E2" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K2" s="37">
         <v>500</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M2" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="N2" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>210</v>
-      </c>
       <c r="P2" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="37"/>
       <c r="R2" s="37"/>
       <c r="S2" s="37"/>
       <c r="T2" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U2" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="V2" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="V2" s="53" t="s">
+      <c r="W2" s="37" t="s">
         <v>326</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="X2" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>328</v>
-      </c>
-      <c r="Y2" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -30035,73 +30032,73 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>323</v>
-      </c>
       <c r="D3" s="37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K3" s="37">
         <v>500</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O3" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P3" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q3" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="R3" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="R3" s="37" t="s">
-        <v>188</v>
-      </c>
       <c r="S3" s="37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="T3" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U3" s="37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V3" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="W3" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="X3" s="37" t="s">
         <v>331</v>
       </c>
-      <c r="W3" s="37" t="s">
-        <v>327</v>
-      </c>
-      <c r="X3" s="37" t="s">
-        <v>332</v>
-      </c>
       <c r="Y3" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -30109,73 +30106,73 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>323</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K4" s="37">
         <v>500</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N4" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P4" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="R4" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="S4" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="S4" s="37" t="s">
-        <v>252</v>
-      </c>
       <c r="T4" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V4" s="53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="W4" s="37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -30209,13 +30206,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>336</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30223,13 +30220,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>338</v>
-      </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -30237,13 +30234,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>338</v>
-      </c>
       <c r="D3" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30251,13 +30248,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>338</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -30286,13 +30283,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>336</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30300,13 +30297,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -30314,13 +30311,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30328,13 +30325,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -30389,67 +30386,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F1" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="K1" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>345</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>346</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q1" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="J1" s="37" t="s">
-        <v>342</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>343</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>345</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>346</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>347</v>
-      </c>
-      <c r="P1" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="R1" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="S1" s="45" t="s">
+      <c r="T1" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="U1" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="V1" s="37" t="s">
         <v>320</v>
-      </c>
-      <c r="V1" s="37" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -30457,67 +30454,67 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>324</v>
-      </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="H2" s="37" t="s">
+      <c r="I2" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="I2" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="K2" s="37" t="s">
+      <c r="L2" s="37" t="s">
         <v>351</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="M2" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="N2" s="37" t="s">
         <v>353</v>
-      </c>
-      <c r="N2" s="37" t="s">
-        <v>354</v>
       </c>
       <c r="O2" s="37" t="s">
         <v>78</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q2" s="37">
         <v>250</v>
       </c>
       <c r="R2" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S2" s="37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="T2" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="U2" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="V2" s="37" t="s">
         <v>328</v>
-      </c>
-      <c r="V2" s="37" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -30546,13 +30543,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>336</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30560,13 +30557,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -30590,13 +30587,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>336</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30604,13 +30601,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -30646,79 +30643,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>138</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>139</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>60</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>64</v>
       </c>
       <c r="H1" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="O1" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="P1" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="Q1" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="T1" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="S1" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="T1" s="37" t="s">
-        <v>156</v>
-      </c>
       <c r="U1" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="V1" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="W1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="W1" s="37" t="s">
+      <c r="X1" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="X1" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="Y1" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z1" s="37" t="s">
         <v>320</v>
-      </c>
-      <c r="Z1" s="37" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
@@ -30729,76 +30726,76 @@
         <v>9</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>75</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>76</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K2" s="37">
         <v>600</v>
       </c>
       <c r="L2" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="N2" s="37" t="s">
         <v>359</v>
       </c>
-      <c r="M2" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="N2" s="37" t="s">
+      <c r="O2" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="P2" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="U2" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="P2" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q2" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="R2" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="S2" s="37" t="s">
+      <c r="V2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="W2" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="U2" s="37" t="s">
+      <c r="X2" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y2" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z2" s="37" t="s">
         <v>362</v>
-      </c>
-      <c r="V2" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="W2" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y2" s="37" t="s">
-        <v>328</v>
-      </c>
-      <c r="Z2" s="37" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -30826,10 +30823,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -30837,10 +30834,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -30855,7 +30852,9 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30870,46 +30869,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>320</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>370</v>
-      </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>375</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -30917,46 +30916,46 @@
         <v>41</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>376</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>378</v>
-      </c>
       <c r="D2" s="37" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>75</v>
       </c>
       <c r="F2" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="I2" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="J2" s="37" t="s">
         <v>380</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>381</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>370</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>382</v>
       </c>
       <c r="K2" s="40">
         <v>44991</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -30971,7 +30970,9 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -31076,27 +31077,27 @@
         <v>81</v>
       </c>
       <c r="C3" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>82</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="H3" s="24" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>86</v>
       </c>
       <c r="I3" s="24"/>
       <c r="J3" s="28" t="s">
         <v>77</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L3" s="29"/>
     </row>
@@ -31105,13 +31106,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>72</v>
@@ -31120,16 +31121,16 @@
         <v>73</v>
       </c>
       <c r="G4" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="I4" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="J4" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>78</v>
@@ -31141,7 +31142,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="32">
         <v>1</v>
@@ -31178,20 +31179,20 @@
         <v>25</v>
       </c>
       <c r="B6" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>85</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>75</v>
@@ -31203,7 +31204,7 @@
         <v>77</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L6" s="29"/>
     </row>
@@ -31212,7 +31213,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="37">
         <v>1</v>
@@ -31227,16 +31228,16 @@
         <v>73</v>
       </c>
       <c r="G7" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="I7" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="J7" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="K7" s="24" t="s">
         <v>78</v>
@@ -31247,7 +31248,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="32">
         <v>1</v>
@@ -31287,13 +31288,13 @@
         <v>38</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="37">
         <v>1</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>72</v>
@@ -31302,16 +31303,16 @@
         <v>73</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="33" t="s">
         <v>75</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>78</v>
@@ -31322,20 +31323,20 @@
         <v>41</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>85</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>75</v>
@@ -31356,13 +31357,13 @@
         <v>49</v>
       </c>
       <c r="B12" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>105</v>
-      </c>
       <c r="D12" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>72</v>
@@ -31377,10 +31378,10 @@
         <v>75</v>
       </c>
       <c r="I12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="37" t="s">
         <v>92</v>
-      </c>
-      <c r="J12" s="37" t="s">
-        <v>93</v>
       </c>
       <c r="K12" s="33" t="s">
         <v>78</v>
@@ -31391,13 +31392,13 @@
         <v>52</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="24" t="s">
         <v>72</v>
@@ -31412,10 +31413,10 @@
         <v>75</v>
       </c>
       <c r="I13" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="K13" s="24" t="s">
         <v>78</v>
@@ -31426,7 +31427,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="37">
         <v>1</v>
@@ -31441,7 +31442,7 @@
         <v>73</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="33" t="s">
         <v>75</v>
@@ -32470,16 +32471,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>385</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -32487,19 +32488,19 @@
         <v>17</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="26"/>
       <c r="B3" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1"/>
@@ -33530,13 +33531,13 @@
         <v>64</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>109</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -33547,13 +33548,13 @@
         <v>75</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -33561,16 +33562,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -33578,16 +33579,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -33598,13 +33599,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -33615,13 +33616,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -33629,16 +33630,16 @@
         <v>32</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -33659,13 +33660,13 @@
         <v>75</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -33676,13 +33677,13 @@
         <v>75</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -33693,13 +33694,13 @@
         <v>75</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -33710,13 +33711,13 @@
         <v>75</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -33727,13 +33728,13 @@
         <v>75</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -33764,31 +33765,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>124</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>125</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>61</v>
@@ -33802,28 +33803,28 @@
         <v>17</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="I2" s="37" t="s">
         <v>132</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>133</v>
       </c>
       <c r="J2" s="37">
         <v>1000</v>
@@ -33840,17 +33841,17 @@
         <v>25</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
       <c r="F3" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G3" s="35"/>
       <c r="H3" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I3" s="42">
         <v>45130</v>
@@ -33873,7 +33874,9 @@
   </sheetPr>
   <dimension ref="A1:AF998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -33899,91 +33902,91 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="O1" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="P1" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="Q1" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="R1" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="S1" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="T1" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="U1" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="V1" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="45" t="s">
+      <c r="W1" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="X1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="Y1" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Z1" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="AA1" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="AA1" s="37" t="s">
+      <c r="AB1" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AB1" s="37" t="s">
+      <c r="AC1" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="AC1" s="37" t="s">
+      <c r="AD1" s="37" t="s">
         <v>164</v>
-      </c>
-      <c r="AD1" s="37" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15.75" customHeight="1">
@@ -33994,79 +33997,79 @@
         <v>9</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>77</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K2" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L2" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="M2" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="N2" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="O2" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="P2" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="Q2" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="R2" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="S2" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="S2" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="T2" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V2" s="37"/>
       <c r="W2" s="37"/>
       <c r="X2" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y2" s="37">
         <v>600</v>
       </c>
       <c r="Z2" s="37"/>
       <c r="AA2" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB2" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC2" s="37" t="s">
         <v>176</v>
-      </c>
-      <c r="AC2" s="37" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15.75" customHeight="1">
@@ -34077,81 +34080,81 @@
         <v>9</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>179</v>
-      </c>
       <c r="G3" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="37"/>
       <c r="J3" s="37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L3" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="N3" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="O3" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="O3" s="37" t="s">
+      <c r="P3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="R3" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S3" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="R3" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="S3" s="37" t="s">
+      <c r="T3" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="V3" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="T3" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="U3" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="V3" s="37" t="s">
+      <c r="W3" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="W3" s="37" t="s">
-        <v>188</v>
-      </c>
       <c r="X3" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Y3" s="37">
         <v>600</v>
       </c>
       <c r="Z3" s="37"/>
       <c r="AA3" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB3" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC3" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AD3" s="37" t="s">
         <v>190</v>
-      </c>
-      <c r="AD3" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" customHeight="1">
@@ -34162,75 +34165,75 @@
         <v>9</v>
       </c>
       <c r="C4" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>193</v>
-      </c>
       <c r="G4" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="37"/>
       <c r="J4" s="37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L4" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="M4" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="N4" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="O4" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="N4" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="O4" s="37" t="s">
+      <c r="P4" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q4" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="P4" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q4" s="37" t="s">
+      <c r="R4" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S4" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="R4" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="S4" s="37" t="s">
-        <v>198</v>
-      </c>
       <c r="T4" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Y4" s="37">
         <v>600</v>
       </c>
       <c r="Z4" s="37"/>
       <c r="AA4" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB4" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC4" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="AC4" s="37" t="s">
+      <c r="AD4" s="37" t="s">
         <v>190</v>
-      </c>
-      <c r="AD4" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="15.75" customHeight="1">
@@ -34241,79 +34244,79 @@
         <v>9</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>76</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L5" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="M5" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="N5" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="O5" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="N5" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="O5" s="37" t="s">
+      <c r="P5" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q5" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="P5" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q5" s="37" t="s">
-        <v>204</v>
-      </c>
       <c r="R5" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S5" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="S5" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="T5" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U5" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V5" s="37"/>
       <c r="W5" s="37"/>
       <c r="X5" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y5" s="37">
         <v>600</v>
       </c>
       <c r="Z5" s="37"/>
       <c r="AA5" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB5" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC5" s="37" t="s">
         <v>176</v>
-      </c>
-      <c r="AC5" s="37" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="15.75" customHeight="1">
@@ -34324,73 +34327,73 @@
         <v>9</v>
       </c>
       <c r="C6" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="37" t="s">
+      <c r="G6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="G6" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="K6" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" s="37" t="s">
+      <c r="M6" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="N6" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="O6" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="N6" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="O6" s="37" t="s">
+      <c r="P6" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q6" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="P6" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q6" s="37" t="s">
+      <c r="R6" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S6" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="R6" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="S6" s="37" t="s">
-        <v>211</v>
-      </c>
       <c r="T6" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U6" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V6" s="37"/>
       <c r="W6" s="37"/>
       <c r="X6" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Y6" s="37">
         <v>600</v>
       </c>
       <c r="Z6" s="37"/>
       <c r="AA6" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB6" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC6" s="37" t="s">
         <v>176</v>
-      </c>
-      <c r="AC6" s="37" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="15.75" customHeight="1">
@@ -34401,79 +34404,79 @@
         <v>9</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>77</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>76</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I7" s="41" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K7" s="41" t="s">
         <v>76</v>
       </c>
       <c r="L7" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="M7" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="N7" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="O7" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="N7" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="O7" s="37" t="s">
+      <c r="P7" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q7" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="P7" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q7" s="41" t="s">
-        <v>216</v>
-      </c>
       <c r="R7" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S7" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="S7" s="41" t="s">
-        <v>175</v>
-      </c>
       <c r="T7" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U7" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V7" s="41"/>
       <c r="W7" s="41"/>
       <c r="X7" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y7" s="37">
         <v>600</v>
       </c>
       <c r="Z7" s="41"/>
       <c r="AA7" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB7" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC7" s="41" t="s">
         <v>176</v>
-      </c>
-      <c r="AC7" s="41" t="s">
-        <v>177</v>
       </c>
       <c r="AD7" s="35"/>
       <c r="AE7" s="35"/>
@@ -34493,76 +34496,76 @@
         <v>9</v>
       </c>
       <c r="C9" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>218</v>
-      </c>
       <c r="G9" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L9" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="M9" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="N9" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="O9" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="N9" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="O9" s="37" t="s">
+      <c r="P9" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="Q9" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="R9" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S9" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="Q9" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="R9" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="S9" s="48" t="s">
-        <v>223</v>
-      </c>
       <c r="T9" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U9" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V9" s="37"/>
       <c r="W9" s="37"/>
       <c r="X9" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Y9" s="37">
         <v>600</v>
       </c>
       <c r="Z9" s="37"/>
       <c r="AA9" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB9" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC9" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="AC9" s="37" t="s">
+      <c r="AD9" s="37" t="s">
         <v>190</v>
-      </c>
-      <c r="AD9" s="37" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="15.75" customHeight="1">
@@ -34573,79 +34576,79 @@
         <v>9</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>77</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K10" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L10" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M10" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="N10" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="O10" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="N10" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="O10" s="37" t="s">
-        <v>228</v>
-      </c>
       <c r="P10" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R10" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S10" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="S10" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="T10" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U10" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V10" s="37"/>
       <c r="W10" s="37"/>
       <c r="X10" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y10" s="37">
         <v>600</v>
       </c>
       <c r="Z10" s="37"/>
       <c r="AA10" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB10" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC10" s="37" t="s">
         <v>176</v>
-      </c>
-      <c r="AC10" s="37" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15.75" customHeight="1">
@@ -34656,73 +34659,73 @@
         <v>9</v>
       </c>
       <c r="C11" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="37" t="s">
+      <c r="G11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="K11" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="37" t="s">
+      <c r="M11" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="N11" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="O11" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="N11" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="O11" s="37" t="s">
+      <c r="P11" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="P11" s="37" t="s">
+      <c r="Q11" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="R11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="S11" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="Q11" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="R11" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="S11" s="48" t="s">
-        <v>235</v>
-      </c>
       <c r="T11" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U11" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V11" s="37"/>
       <c r="W11" s="37"/>
       <c r="X11" s="37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y11" s="37">
         <v>600</v>
       </c>
       <c r="Z11" s="37"/>
       <c r="AA11" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB11" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC11" s="41" t="s">
         <v>176</v>
-      </c>
-      <c r="AC11" s="41" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="15.75" customHeight="1">
@@ -34733,74 +34736,74 @@
         <v>9</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="D12" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>237</v>
-      </c>
       <c r="G12" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K12" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L12" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="M12" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="M12" s="37" t="s">
+      <c r="N12" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="O12" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="N12" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="O12" s="37" t="s">
+      <c r="P12" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="P12" s="37" t="s">
+      <c r="Q12" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="R12" s="37" t="s">
         <v>241</v>
-      </c>
-      <c r="Q12" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="R12" s="37" t="s">
-        <v>242</v>
       </c>
       <c r="S12" s="48"/>
       <c r="T12" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U12" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V12" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="W12" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="W12" s="37" t="s">
-        <v>188</v>
-      </c>
       <c r="X12" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Y12" s="37">
         <v>600</v>
       </c>
       <c r="Z12" s="37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AB12" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC12" s="41" t="s">
         <v>176</v>
-      </c>
-      <c r="AC12" s="41" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="15.75" customHeight="1">
@@ -34811,74 +34814,74 @@
         <v>9</v>
       </c>
       <c r="C13" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="D13" s="46" t="s">
-        <v>244</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>245</v>
-      </c>
       <c r="G13" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K13" s="37" t="s">
         <v>76</v>
       </c>
       <c r="L13" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="M13" s="46" t="s">
         <v>246</v>
       </c>
-      <c r="M13" s="46" t="s">
+      <c r="N13" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="O13" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="N13" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="O13" s="37" t="s">
+      <c r="P13" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="P13" s="37" t="s">
-        <v>249</v>
-      </c>
       <c r="Q13" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R13" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="S13" s="46"/>
       <c r="T13" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U13" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V13" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="W13" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W13" s="37" t="s">
-        <v>251</v>
-      </c>
       <c r="X13" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y13" s="37">
         <v>600</v>
       </c>
       <c r="Z13" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AB13" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC13" s="41" t="s">
         <v>176</v>
-      </c>
-      <c r="AC13" s="41" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="15.75" customHeight="1"/>
@@ -35881,7 +35884,7 @@
   </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -35906,82 +35909,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>258</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="N1" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="O1" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="P1" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="Q1" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="U1" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="V1" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="W1" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="R1" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="S1" s="37" t="s">
+      <c r="Y1" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="T1" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="U1" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="V1" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="W1" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="X1" s="37" t="s">
+      <c r="Z1" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="Y1" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z1" s="37" t="s">
+      <c r="AA1" s="37" t="s">
         <v>268</v>
-      </c>
-      <c r="AA1" s="37" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -35989,151 +35992,151 @@
         <v>17</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="L2" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="L2" s="37" t="s">
+      <c r="M2" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="O2" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="O2" s="37" t="s">
-        <v>275</v>
-      </c>
       <c r="Q2" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R2" s="37">
         <v>400</v>
       </c>
       <c r="S2" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="V2" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="W2" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="X2" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="T2" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="U2" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="V2" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="W2" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>277</v>
-      </c>
       <c r="Y2" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z2" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA2" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="37" t="s">
+      <c r="L3" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="M3" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="P3" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="J3" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="L3" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>130</v>
-      </c>
-      <c r="Q3" s="37" t="s">
-        <v>131</v>
       </c>
       <c r="R3" s="37">
         <v>400</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T3" s="37"/>
       <c r="U3" s="37"/>
       <c r="V3" s="37"/>
       <c r="W3" s="37"/>
       <c r="X3" s="37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y3" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z3" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA3" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -36141,82 +36144,82 @@
         <v>25</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>269</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="L4" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>270</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="K4" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="L4" s="41" t="s">
-        <v>284</v>
-      </c>
       <c r="M4" s="41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P4" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q4" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R4" s="43">
         <v>600</v>
       </c>
       <c r="S4" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U4" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="V4" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="V4" s="37" t="s">
-        <v>203</v>
-      </c>
       <c r="W4" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y4" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z4" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA4" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -36224,76 +36227,76 @@
         <v>38</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C5" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="41" t="s">
+      <c r="G5" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="M5" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="G5" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>288</v>
-      </c>
       <c r="O5" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q5" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R5" s="37">
         <v>17800</v>
       </c>
       <c r="S5" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="T5" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="U5" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="V5" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="W5" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="X5" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="T5" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="U5" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="V5" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="W5" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="X5" s="37" t="s">
-        <v>290</v>
-      </c>
       <c r="Y5" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z5" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA5" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -36301,82 +36304,82 @@
         <v>41</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="L6" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="G6" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="K6" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>273</v>
-      </c>
       <c r="M6" s="41" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N6" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P6" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q6" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R6" s="43">
         <v>500</v>
       </c>
       <c r="S6" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T6" s="37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U6" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="V6" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V6" s="37" t="s">
-        <v>228</v>
-      </c>
       <c r="W6" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X6" s="37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y6" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z6" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA6" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -36384,76 +36387,76 @@
         <v>49</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C7" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q7" s="41" t="s">
         <v>292</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="L7" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="M7" s="37" t="s">
-        <v>288</v>
-      </c>
-      <c r="O7" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q7" s="41" t="s">
-        <v>293</v>
       </c>
       <c r="R7" s="37">
         <v>2000</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T7" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U7" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="V7" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="V7" s="37" t="s">
-        <v>233</v>
-      </c>
       <c r="W7" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X7" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Y7" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z7" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA7" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -36483,50 +36486,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="D1" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>298</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="172.5" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B2" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="E2" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>303</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="100.5" customHeight="1">
       <c r="A3" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -36574,73 +36577,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="G1" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="I1" s="37" t="s">
+      <c r="K1" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="J1" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="L1" s="37" t="s">
-        <v>309</v>
-      </c>
       <c r="M1" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="O1" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="P1" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="Q1" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="S1" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="S1" s="37" t="s">
-        <v>266</v>
-      </c>
       <c r="T1" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="V1" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="V1" s="37" t="s">
-        <v>155</v>
-      </c>
       <c r="W1" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="X1" s="37" t="s">
         <v>268</v>
-      </c>
-      <c r="X1" s="37" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -36648,73 +36651,73 @@
         <v>21</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>270</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>311</v>
-      </c>
       <c r="J2" s="41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K2" s="41" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M2" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O2" s="41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P2" s="41" t="s">
         <v>73</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R2" s="41" t="s">
         <v>73</v>
       </c>
       <c r="S2" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T2" s="43">
         <v>500</v>
       </c>
       <c r="U2" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="V2" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W2" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X2" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated basic details and excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/upp-automation-testdata.xlsx
+++ b/src/main/resources/upp-automation-testdata.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="397">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -155,6 +155,9 @@
     <t>In Progress</t>
   </si>
   <si>
+    <t>30-03-2023</t>
+  </si>
+  <si>
     <t>TS06</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
   <si>
     <t>ECommerce Transaction + Party API + Transaction API (REST API calls)
 Depends on TS07</t>
+  </si>
+  <si>
+    <t>31-03-2023</t>
   </si>
   <si>
     <t>TS09</t>
@@ -232,9 +238,6 @@
     <t xml:space="preserve">Create a Deal with  1 party and then Add another Party through Api and Use The GET Party Api and Update Party API
  and  then edit the live deal and create a transaction using Payment Tab in Scheduled Instruction
 </t>
-  </si>
-  <si>
-    <t>29-03-2023</t>
   </si>
   <si>
     <t>TS12</t>
@@ -1257,9 +1260,6 @@
   </si>
   <si>
     <t>PartyABCD</t>
-  </si>
-  <si>
-    <t>Adhoc Payment1</t>
   </si>
   <si>
     <t>Creditorpartyid123</t>
@@ -2253,7 +2253,9 @@
       <c r="H7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -2275,14 +2277,14 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="6" t="s">
@@ -2313,14 +2315,14 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="6" t="s">
@@ -2351,14 +2353,14 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="6" t="s">
@@ -2367,7 +2369,9 @@
       <c r="H10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2389,16 +2393,16 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="6" t="s">
@@ -2429,16 +2433,16 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="6" t="s">
@@ -2448,7 +2452,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -2471,19 +2475,19 @@
     <row r="13" ht="68.25" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>12</v>
@@ -2492,7 +2496,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -2515,16 +2519,16 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="6" t="s">
@@ -2534,7 +2538,7 @@
         <v>31</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -2557,14 +2561,14 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="6" t="s">
@@ -2574,7 +2578,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -2597,14 +2601,14 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="6" t="s">
@@ -2614,7 +2618,7 @@
         <v>13</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -30051,295 +30055,295 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L1" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="42" t="s">
-        <v>149</v>
-      </c>
-      <c r="N1" s="42" t="s">
-        <v>147</v>
-      </c>
       <c r="O1" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="P1" s="43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="43" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R1" s="43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="S1" s="43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="T1" s="43" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="U1" s="43" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Y1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K2" s="35">
         <v>500.0</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M2" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="N2" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="N2" s="35" t="s">
-        <v>207</v>
-      </c>
       <c r="O2" s="35" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="35"/>
       <c r="R2" s="35"/>
       <c r="S2" s="35"/>
       <c r="T2" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="V2" s="56" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="W2" s="35" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X2" s="35" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Y2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I3" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="35" t="s">
         <v>241</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>240</v>
       </c>
       <c r="K3" s="35">
         <v>500.0</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M3" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="N3" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="N3" s="35" t="s">
-        <v>238</v>
-      </c>
       <c r="O3" s="35" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R3" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="T3" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U3" s="35" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="V3" s="56" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="W3" s="35" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X3" s="35" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Y3" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K4" s="35">
         <v>500.0</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M4" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="N4" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="N4" s="44" t="s">
-        <v>246</v>
-      </c>
       <c r="O4" s="39" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="V4" s="56" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="W4" s="35" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="X4" s="35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Y4" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30372,55 +30376,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30448,55 +30452,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30549,99 +30553,99 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="S1" s="43" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>357</v>
+        <v>270</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>358</v>
       </c>
       <c r="I2" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="35" t="s">
         <v>111</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>110</v>
       </c>
       <c r="K2" s="35" t="s">
         <v>359</v>
@@ -30656,7 +30660,7 @@
         <v>362</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P2" s="35" t="s">
         <v>363</v>
@@ -30665,19 +30669,19 @@
         <v>250.0</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30705,27 +30709,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>364</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30748,27 +30752,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -30803,84 +30807,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K1" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q1" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="S1" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="U1" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="N1" s="42" t="s">
-        <v>149</v>
-      </c>
-      <c r="O1" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="P1" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="S1" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>158</v>
-      </c>
       <c r="V1" s="35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y1" s="35" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Z1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>9</v>
@@ -30892,19 +30896,19 @@
         <v>365</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>365</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J2" s="35" t="s">
         <v>366</v>
@@ -30916,7 +30920,7 @@
         <v>367</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N2" s="35" t="s">
         <v>368</v>
@@ -30925,34 +30929,34 @@
         <v>369</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U2" s="35" t="s">
         <v>370</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="W2" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="X2" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Y2" s="35" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Z2" s="35" t="s">
         <v>371</v>
@@ -30982,18 +30986,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>372</v>
@@ -31040,7 +31044,7 @@
         <v>377</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H1" s="35" t="s">
         <v>378</v>
@@ -31069,7 +31073,7 @@
     </row>
     <row r="2">
       <c r="A2" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>385</v>
@@ -31081,7 +31085,7 @@
         <v>387</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>377</v>
@@ -31145,40 +31149,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -31186,40 +31190,40 @@
         <v>8</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="22">
         <v>1.0</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -31227,30 +31231,30 @@
         <v>14</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L3" s="27"/>
     </row>
@@ -31259,34 +31263,34 @@
         <v>17</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" s="26">
         <v>1.0</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L4" s="27"/>
     </row>
@@ -31295,34 +31299,34 @@
         <v>21</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="30">
         <v>1.0</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L5" s="32"/>
       <c r="M5" s="33"/>
@@ -31332,282 +31336,282 @@
         <v>25</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L6" s="27"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C7" s="35">
         <v>1.0</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C8" s="30">
         <v>1.0</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C10" s="35">
         <v>1.0</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L11" s="27"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>104</v>
-      </c>
       <c r="D13" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" s="35">
         <v>1.0</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K14" s="31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1"/>
@@ -32640,16 +32644,16 @@
         <v>17</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>396</v>
@@ -33679,16 +33683,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2">
@@ -33696,16 +33700,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
@@ -33713,16 +33717,16 @@
         <v>14</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4">
@@ -33730,16 +33734,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
@@ -33747,16 +33751,16 @@
         <v>21</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
@@ -33764,128 +33768,140 @@
         <v>25</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -33915,37 +33931,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -33953,28 +33969,28 @@
         <v>17</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J2" s="35">
         <v>1000.0</v>
@@ -33991,17 +34007,17 @@
         <v>25</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="39" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I3" s="40">
         <v>45130.0</v>
@@ -34049,91 +34065,91 @@
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N1" s="42" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O1" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P1" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Q1" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T1" s="43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="V1" s="43" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="W1" s="43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Y1" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Z1" s="43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AA1" s="35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AB1" s="35" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AC1" s="35" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD1" s="35" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -34144,79 +34160,79 @@
         <v>9</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F2" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>166</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>165</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="N2" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P2" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V2" s="35"/>
       <c r="W2" s="35"/>
       <c r="X2" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y2" s="35">
         <v>600.0</v>
       </c>
       <c r="Z2" s="35"/>
       <c r="AA2" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB2" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC2" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -34227,81 +34243,81 @@
         <v>9</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E3" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="H3" s="35"/>
       <c r="J3" s="35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M3" s="44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q3" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="S3" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="U3" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="W3" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="X3" s="35" t="s">
         <v>184</v>
-      </c>
-      <c r="R3" s="35" t="s">
-        <v>173</v>
-      </c>
-      <c r="S3" s="35" t="s">
-        <v>185</v>
-      </c>
-      <c r="T3" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="U3" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="V3" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="W3" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="X3" s="35" t="s">
-        <v>183</v>
       </c>
       <c r="Y3" s="35">
         <v>600.0</v>
       </c>
       <c r="Z3" s="35"/>
       <c r="AA3" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AB3" s="35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC3" s="35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AD3" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -34312,75 +34328,75 @@
         <v>9</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E4" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>92</v>
       </c>
       <c r="H4" s="35"/>
       <c r="J4" s="35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="X4" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y4" s="35">
         <v>600.0</v>
       </c>
       <c r="Z4" s="35"/>
       <c r="AA4" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AB4" s="35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC4" s="35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AD4" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -34391,239 +34407,239 @@
         <v>9</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E5" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="H5" s="35" t="s">
         <v>199</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>198</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M5" s="44" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P5" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q5" s="35" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T5" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V5" s="35"/>
       <c r="W5" s="35"/>
       <c r="X5" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y5" s="35">
         <v>600.0</v>
       </c>
       <c r="Z5" s="35"/>
       <c r="AA5" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB5" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC5" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E6" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="J6" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>204</v>
-      </c>
       <c r="K6" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P6" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q6" s="35" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="R6" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S6" s="35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="T6" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U6" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V6" s="35"/>
       <c r="W6" s="35"/>
       <c r="X6" s="35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y6" s="35">
         <v>600.0</v>
       </c>
       <c r="Z6" s="35"/>
       <c r="AA6" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AB6" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC6" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>76</v>
-      </c>
       <c r="H7" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I7" s="39" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L7" s="45" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N7" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O7" s="35" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="P7" s="39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q7" s="39" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="R7" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S7" s="39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T7" s="39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U7" s="39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V7" s="39"/>
       <c r="W7" s="39"/>
       <c r="X7" s="39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y7" s="35">
         <v>600.0</v>
       </c>
       <c r="Z7" s="39"/>
       <c r="AA7" s="39" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB7" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC7" s="39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AD7" s="33"/>
       <c r="AE7" s="33"/>
@@ -34631,404 +34647,404 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O8" s="35"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F9" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="G9" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>216</v>
-      </c>
       <c r="K9" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M9" s="44" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N9" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P9" s="35" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Q9" s="35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="R9" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S9" s="46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="T9" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U9" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V9" s="35"/>
       <c r="W9" s="35"/>
       <c r="X9" s="35" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Y9" s="35">
         <v>600.0</v>
       </c>
       <c r="Z9" s="35"/>
       <c r="AA9" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB9" s="35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC9" s="35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AD9" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F10" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="35" t="s">
         <v>224</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>223</v>
       </c>
       <c r="I10" s="35" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K10" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N10" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O10" s="35" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P10" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q10" s="35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="R10" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S10" s="35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T10" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U10" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="35"/>
       <c r="W10" s="35"/>
       <c r="X10" s="35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y10" s="35">
         <v>600.0</v>
       </c>
       <c r="Z10" s="35"/>
       <c r="AA10" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB10" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC10" s="35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E11" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="J11" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="G11" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>228</v>
-      </c>
       <c r="K11" s="35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M11" s="44" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N11" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O11" s="35" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P11" s="35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Q11" s="35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="R11" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S11" s="46" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="T11" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U11" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V11" s="35"/>
       <c r="W11" s="35"/>
       <c r="X11" s="35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Y11" s="35">
         <v>600.0</v>
       </c>
       <c r="Z11" s="35"/>
       <c r="AA11" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB11" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC11" s="39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E12" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="G12" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="J12" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="G12" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>235</v>
-      </c>
       <c r="K12" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="N12" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O12" s="35" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P12" s="35" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Q12" s="35" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="R12" s="35" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="S12" s="46"/>
       <c r="T12" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U12" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W12" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="X12" s="35" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Y12" s="35">
         <v>600.0</v>
       </c>
       <c r="Z12" s="35" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AB12" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC12" s="39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E13" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="G13" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="J13" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>243</v>
-      </c>
       <c r="K13" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M13" s="44" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P13" s="35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Q13" s="39" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="R13" s="35" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="S13" s="44"/>
       <c r="T13" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U13" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V13" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="W13" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="X13" s="35" t="s">
         <v>249</v>
-      </c>
-      <c r="W13" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="X13" s="35" t="s">
-        <v>248</v>
       </c>
       <c r="Y13" s="35">
         <v>600.0</v>
       </c>
       <c r="Z13" s="35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AB13" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC13" s="39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1"/>
@@ -36053,82 +36069,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T1" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U1" s="42" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="V1" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="W1" s="42" t="s">
-        <v>148</v>
-      </c>
       <c r="X1" s="35" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Y1" s="35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Z1" s="35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AA1" s="35" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
@@ -36136,151 +36152,151 @@
         <v>17</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C2" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>269</v>
-      </c>
       <c r="E2" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M2" s="35" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R2" s="35">
         <v>400.0</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="T2" s="35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="V2" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="W2" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="W2" s="35" t="s">
-        <v>181</v>
-      </c>
       <c r="X2" s="35" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Y2" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Z2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA2" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="37" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>269</v>
-      </c>
       <c r="E3" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>271</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>272</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>279</v>
-      </c>
-      <c r="N3" s="35" t="s">
-        <v>125</v>
-      </c>
       <c r="O3" s="35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q3" s="35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R3" s="35">
         <v>400.0</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="T3" s="35"/>
       <c r="U3" s="35"/>
       <c r="V3" s="35"/>
       <c r="W3" s="35"/>
       <c r="X3" s="35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="Y3" s="35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Z3" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA3" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4">
@@ -36288,319 +36304,319 @@
         <v>25</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E4" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="N4" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="K4" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="L4" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="N4" s="39" t="s">
-        <v>125</v>
-      </c>
       <c r="O4" s="39" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P4" s="39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q4" s="39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R4" s="41">
         <v>600.0</v>
       </c>
       <c r="S4" s="39" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="T4" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="U4" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="V4" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="U4" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="V4" s="35" t="s">
-        <v>202</v>
-      </c>
       <c r="W4" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="X4" s="35" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y4" s="39" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Z4" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA4" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q5" s="39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R5" s="35">
         <v>17800.0</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="T5" s="35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="V5" s="35" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="W5" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X5" s="35" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y5" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA5" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="39" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E6" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="N6" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="K6" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>272</v>
-      </c>
-      <c r="M6" s="39" t="s">
-        <v>290</v>
-      </c>
-      <c r="N6" s="39" t="s">
-        <v>125</v>
-      </c>
       <c r="O6" s="39" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P6" s="39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q6" s="39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R6" s="41">
         <v>500.0</v>
       </c>
       <c r="S6" s="39" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="T6" s="35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U6" s="35" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="V6" s="35" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="W6" s="35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="X6" s="35" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Y6" s="39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z6" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA6" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K7" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O7" s="35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q7" s="39" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="R7" s="35">
         <v>2000.0</v>
       </c>
       <c r="S7" s="35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="T7" s="35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="U7" s="35" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="V7" s="35" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="W7" s="35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X7" s="35" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Y7" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA7" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -36632,77 +36648,77 @@
         <v>0</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" ht="172.5" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" ht="100.5" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F3" s="51"/>
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5">
@@ -36779,19 +36795,19 @@
   <sheetData>
     <row r="1" ht="172.5" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
@@ -36865,73 +36881,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="P1" s="43" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="W1" s="35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="X1" s="35" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
@@ -36939,73 +36955,73 @@
         <v>21</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K2" s="39" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S2" s="39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T2" s="41">
         <v>500.0</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="V2" s="39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="W2" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="X2" s="39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>